<commit_message>
added rallyx driver. Missing only samples support
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17811" uniqueCount="4688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17812" uniqueCount="4692">
   <si>
     <t>TODO</t>
   </si>
@@ -14115,6 +14115,18 @@
   </si>
   <si>
     <t>10 Yard Fight (Vs. version set 2)</t>
+  </si>
+  <si>
+    <t>Rally X</t>
+  </si>
+  <si>
+    <t>Rally X (Midway)</t>
+  </si>
+  <si>
+    <t>New Rally X</t>
+  </si>
+  <si>
+    <t>no sample support</t>
   </si>
 </sst>
 </file>
@@ -14955,7 +14967,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14990,7 +15002,7 @@
         <v>4638</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -15000,7 +15012,7 @@
       </c>
       <c r="E3">
         <f>B3*100/D3</f>
-        <v>0.39043435822352368</v>
+        <v>0.53684724255734506</v>
       </c>
       <c r="F3" t="s">
         <v>4439</v>
@@ -15158,7 +15170,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -15168,7 +15180,7 @@
       </c>
       <c r="E11">
         <f>B11*100/D11</f>
-        <v>81.405563689604691</v>
+        <v>81.259150805270863</v>
       </c>
       <c r="F11" t="s">
         <v>4439</v>
@@ -15406,8 +15418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1717"/>
   <sheetViews>
-    <sheetView topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="A396" sqref="A396:XFD401"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:XFD118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18593,90 +18605,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B116">
-        <v>113</v>
-      </c>
-      <c r="C116" t="s">
-        <v>444</v>
-      </c>
-      <c r="D116" t="s">
-        <v>445</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J116" t="s">
-        <v>436</v>
-      </c>
-      <c r="M116" t="s">
-        <v>446</v>
-      </c>
-      <c r="N116" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B117">
-        <v>114</v>
-      </c>
-      <c r="C117" t="s">
-        <v>447</v>
-      </c>
-      <c r="D117" t="s">
-        <v>445</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I117" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J117" t="s">
-        <v>436</v>
-      </c>
-      <c r="M117" t="s">
-        <v>446</v>
-      </c>
-      <c r="N117" t="s">
-        <v>98</v>
-      </c>
-      <c r="O117" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B118">
-        <v>115</v>
-      </c>
-      <c r="C118" t="s">
-        <v>448</v>
-      </c>
-      <c r="D118" t="s">
-        <v>445</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J118" t="s">
-        <v>436</v>
-      </c>
-      <c r="M118" t="s">
-        <v>39</v>
-      </c>
-      <c r="N118" t="s">
-        <v>446</v>
-      </c>
-      <c r="O118" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="119" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>116</v>
@@ -71616,7 +71544,7 @@
   <dimension ref="A1:L335"/>
   <sheetViews>
     <sheetView topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="A336" sqref="A336"/>
+      <selection activeCell="A336" sqref="A336:XFD338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -80397,10 +80325,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -80671,6 +80599,99 @@
       </c>
       <c r="L9" t="s">
         <v>4661</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4632</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>444</v>
+      </c>
+      <c r="D10" t="s">
+        <v>445</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>436</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4688</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4632</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>447</v>
+      </c>
+      <c r="D11" t="s">
+        <v>445</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>436</v>
+      </c>
+      <c r="K11" t="s">
+        <v>4689</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4632</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" t="s">
+        <v>445</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>436</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4690</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added working sauro driver
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -15056,7 +15056,7 @@
         <v>4271</v>
       </c>
       <c r="B2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -15066,7 +15066,7 @@
       </c>
       <c r="E2">
         <f>B2*100/D2</f>
-        <v>18.399219131283552</v>
+        <v>18.448023426061493</v>
       </c>
       <c r="F2" t="s">
         <v>4373</v>
@@ -15245,7 +15245,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -15255,7 +15255,7 @@
       </c>
       <c r="E11">
         <f>B11*100/D11</f>
-        <v>77.257198633479746</v>
+        <v>77.208394338701808</v>
       </c>
       <c r="F11" t="s">
         <v>4373</v>
@@ -15493,8 +15493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1634"/>
   <sheetViews>
-    <sheetView topLeftCell="A902" workbookViewId="0">
-      <selection activeCell="A914" sqref="A914:XFD915"/>
+    <sheetView topLeftCell="A1437" workbookViewId="0">
+      <selection activeCell="A1452" sqref="A1452:XFD1452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63415,32 +63415,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="1452" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1452">
-        <v>1450</v>
-      </c>
-      <c r="C1452" t="s">
-        <v>3869</v>
-      </c>
-      <c r="D1452" t="s">
-        <v>3870</v>
-      </c>
-      <c r="E1452" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1452" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1452" t="s">
-        <v>167</v>
-      </c>
-      <c r="I1452" t="s">
-        <v>353</v>
-      </c>
-      <c r="J1452" t="s">
-        <v>3871</v>
-      </c>
-    </row>
     <row r="1453" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1453">
         <v>1451</v>
@@ -68773,10 +68747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L378"/>
+  <dimension ref="A1:L379"/>
   <sheetViews>
     <sheetView topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="L377" sqref="L377:M378"/>
+      <selection activeCell="A380" sqref="A380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78806,6 +78780,32 @@
       </c>
       <c r="K378" t="s">
         <v>4715</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>4636</v>
+      </c>
+      <c r="B379">
+        <v>378</v>
+      </c>
+      <c r="C379" t="s">
+        <v>3869</v>
+      </c>
+      <c r="D379" t="s">
+        <v>3870</v>
+      </c>
+      <c r="E379" t="s">
+        <v>10</v>
+      </c>
+      <c r="F379" t="s">
+        <v>4260</v>
+      </c>
+      <c r="H379" t="s">
+        <v>353</v>
+      </c>
+      <c r="K379" t="s">
+        <v>3871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added double dragon working driver (no stereo output though) + a few more small fixes to other drivers
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17634" uniqueCount="4746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17630" uniqueCount="4750">
   <si>
     <t>TODO</t>
   </si>
@@ -14289,6 +14289,18 @@
   </si>
   <si>
     <t>Nebulous Bee</t>
+  </si>
+  <si>
+    <t>Double Dragon</t>
+  </si>
+  <si>
+    <t>Double Dragon (bootleg)</t>
+  </si>
+  <si>
+    <t>Double Dragon II - The Revenge</t>
+  </si>
+  <si>
+    <t>no stereo support</t>
   </si>
 </sst>
 </file>
@@ -15131,7 +15143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -15839,8 +15851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1525"/>
   <sheetViews>
-    <sheetView topLeftCell="A1453" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B1480"/>
+    <sheetView topLeftCell="A1166" workbookViewId="0">
+      <selection activeCell="A1182" sqref="A1182:XFD1183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54615,7 +54627,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="1169" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1169" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1169">
         <v>1165</v>
       </c>
@@ -54650,7 +54662,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="1170" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1170" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1170">
         <v>1166</v>
       </c>
@@ -54685,7 +54697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1171" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1171" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1171">
         <v>1167</v>
       </c>
@@ -54717,7 +54729,7 @@
         <v>3313</v>
       </c>
     </row>
-    <row r="1172" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1172" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1172">
         <v>1168</v>
       </c>
@@ -54749,7 +54761,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="1173" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1173" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1173">
         <v>1169</v>
       </c>
@@ -54790,7 +54802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1174" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1174" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1174">
         <v>1170</v>
       </c>
@@ -54831,7 +54843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1175" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1175" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1175">
         <v>1171</v>
       </c>
@@ -54863,7 +54875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1176" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1176" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1176">
         <v>1172</v>
       </c>
@@ -54901,7 +54913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1177" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1177" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1177">
         <v>1173</v>
       </c>
@@ -54942,7 +54954,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="1178" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1178" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1178">
         <v>1174</v>
       </c>
@@ -54980,7 +54992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1179" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1179" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1179">
         <v>1175</v>
       </c>
@@ -55018,7 +55030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1180" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1180" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1180">
         <v>1176</v>
       </c>
@@ -55056,121 +55068,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="1181" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1181">
-        <v>1177</v>
-      </c>
-      <c r="C1181" t="s">
-        <v>3336</v>
-      </c>
-      <c r="D1181" t="s">
-        <v>3337</v>
-      </c>
-      <c r="E1181" t="s">
-        <v>2338</v>
-      </c>
-      <c r="F1181" t="s">
-        <v>497</v>
-      </c>
-      <c r="G1181" t="s">
-        <v>3338</v>
-      </c>
-      <c r="I1181" t="s">
-        <v>515</v>
-      </c>
-      <c r="J1181" t="s">
-        <v>3339</v>
-      </c>
-      <c r="K1181" t="s">
-        <v>766</v>
-      </c>
-      <c r="L1181" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="1182" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1182">
-        <v>1178</v>
-      </c>
-      <c r="C1182" t="s">
-        <v>3340</v>
-      </c>
-      <c r="D1182" t="s">
-        <v>3337</v>
-      </c>
-      <c r="E1182" t="s">
-        <v>2338</v>
-      </c>
-      <c r="F1182" t="s">
-        <v>2338</v>
-      </c>
-      <c r="G1182" t="s">
-        <v>3338</v>
-      </c>
-      <c r="I1182" t="s">
-        <v>515</v>
-      </c>
-      <c r="J1182" t="s">
-        <v>3339</v>
-      </c>
-      <c r="K1182" t="s">
-        <v>766</v>
-      </c>
-      <c r="L1182" t="s">
-        <v>503</v>
-      </c>
-      <c r="M1182" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="1183" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1183">
-        <v>1179</v>
-      </c>
-      <c r="C1183" t="s">
-        <v>3341</v>
-      </c>
-      <c r="D1183" t="s">
-        <v>3337</v>
-      </c>
-      <c r="E1183" t="s">
-        <v>2338</v>
-      </c>
-      <c r="F1183" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1183" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1183" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1183" t="s">
-        <v>515</v>
-      </c>
-      <c r="K1183" t="s">
-        <v>1557</v>
-      </c>
-      <c r="L1183" t="s">
-        <v>766</v>
-      </c>
-      <c r="M1183" t="s">
-        <v>503</v>
-      </c>
-      <c r="N1183" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1183" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1183" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1183" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="1184" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1184" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1184">
         <v>1180</v>
       </c>
@@ -77369,10 +77267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77380,7 +77278,7 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="13" width="107" bestFit="1" customWidth="1"/>
   </cols>
@@ -78196,6 +78094,76 @@
       </c>
       <c r="M24" t="s">
         <v>4731</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4644</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3340</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3337</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2338</v>
+      </c>
+      <c r="G25" t="s">
+        <v>3338</v>
+      </c>
+      <c r="H25" t="s">
+        <v>515</v>
+      </c>
+      <c r="I25" t="s">
+        <v>3339</v>
+      </c>
+      <c r="K25" t="s">
+        <v>4747</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4644</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3341</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3337</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4190</v>
+      </c>
+      <c r="H26" t="s">
+        <v>515</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1557</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4748</v>
+      </c>
+      <c r="M26" t="s">
+        <v>4749</v>
       </c>
     </row>
   </sheetData>
@@ -81062,10 +81030,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A27"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -81852,6 +81820,38 @@
         <v>4724</v>
       </c>
     </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4644</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3336</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3337</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F29" t="s">
+        <v>497</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3338</v>
+      </c>
+      <c r="I29" t="s">
+        <v>515</v>
+      </c>
+      <c r="J29" t="s">
+        <v>3339</v>
+      </c>
+      <c r="M29" t="s">
+        <v>4746</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated congo and zaxxon drivers to fully playable status
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17563" uniqueCount="4785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17556" uniqueCount="4786">
   <si>
     <t>TODO</t>
   </si>
@@ -14406,6 +14406,9 @@
   </si>
   <si>
     <t>Snow Bros - Nick &amp; Tom (Japan)</t>
+  </si>
+  <si>
+    <t>0.36.13</t>
   </si>
 </sst>
 </file>
@@ -63707,10 +63710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M454"/>
+  <dimension ref="A1:M461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="R450" sqref="R450"/>
+    <sheetView topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="M453" sqref="M453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75769,6 +75772,179 @@
         <v>4780</v>
       </c>
     </row>
+    <row r="455" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B455">
+        <v>454</v>
+      </c>
+      <c r="C455" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D455" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E455" t="s">
+        <v>10</v>
+      </c>
+      <c r="I455" t="s">
+        <v>412</v>
+      </c>
+      <c r="L455" t="s">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="456" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B456">
+        <v>455</v>
+      </c>
+      <c r="C456" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D456" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E456" t="s">
+        <v>10</v>
+      </c>
+      <c r="I456" t="s">
+        <v>412</v>
+      </c>
+      <c r="L456" t="s">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="457" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B457">
+        <v>456</v>
+      </c>
+      <c r="C457" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D457" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E457" t="s">
+        <v>10</v>
+      </c>
+      <c r="I457" t="s">
+        <v>412</v>
+      </c>
+      <c r="L457" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="458" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B458">
+        <v>457</v>
+      </c>
+      <c r="C458" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D458" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E458" t="s">
+        <v>10</v>
+      </c>
+      <c r="I458" t="s">
+        <v>412</v>
+      </c>
+      <c r="L458" t="s">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="459" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B459">
+        <v>458</v>
+      </c>
+      <c r="C459" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D459" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E459" t="s">
+        <v>10</v>
+      </c>
+      <c r="I459" t="s">
+        <v>412</v>
+      </c>
+      <c r="L459" t="s">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="460" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B460">
+        <v>459</v>
+      </c>
+      <c r="C460" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D460" t="s">
+        <v>2007</v>
+      </c>
+      <c r="E460" t="s">
+        <v>10</v>
+      </c>
+      <c r="F460" t="s">
+        <v>4145</v>
+      </c>
+      <c r="I460" t="s">
+        <v>77</v>
+      </c>
+      <c r="J460" t="s">
+        <v>412</v>
+      </c>
+      <c r="L460" t="s">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="461" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>4785</v>
+      </c>
+      <c r="B461">
+        <v>460</v>
+      </c>
+      <c r="C461" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D461" t="s">
+        <v>2007</v>
+      </c>
+      <c r="E461" t="s">
+        <v>10</v>
+      </c>
+      <c r="F461" t="s">
+        <v>4145</v>
+      </c>
+      <c r="I461" t="s">
+        <v>77</v>
+      </c>
+      <c r="J461" t="s">
+        <v>412</v>
+      </c>
+      <c r="L461" t="s">
+        <v>4537</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -75777,10 +75953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:A55"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76234,72 +76410,78 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4518</v>
+        <v>4599</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>2006</v>
+        <v>2560</v>
       </c>
       <c r="D15" t="s">
-        <v>2007</v>
+        <v>2561</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>4145</v>
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>333</v>
       </c>
       <c r="I15" t="s">
-        <v>412</v>
+        <v>736</v>
       </c>
       <c r="K15" t="s">
-        <v>4536</v>
+        <v>4618</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>4506</v>
+        <v>4619</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4518</v>
+        <v>4599</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>2008</v>
+        <v>446</v>
       </c>
       <c r="D16" t="s">
-        <v>2007</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H16" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" t="s">
+        <v>447</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>412</v>
       </c>
       <c r="K16" t="s">
-        <v>4537</v>
+        <v>4694</v>
       </c>
       <c r="L16">
         <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>4506</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -76310,34 +76492,34 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>2560</v>
+        <v>449</v>
       </c>
       <c r="D17" t="s">
-        <v>2561</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" t="s">
-        <v>333</v>
-      </c>
-      <c r="I17" t="s">
-        <v>736</v>
+        <v>447</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="K17" t="s">
-        <v>4618</v>
+        <v>4696</v>
       </c>
       <c r="L17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>4619</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -76348,7 +76530,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D18" t="s">
         <v>447</v>
@@ -76369,7 +76551,7 @@
         <v>412</v>
       </c>
       <c r="K18" t="s">
-        <v>4694</v>
+        <v>4699</v>
       </c>
       <c r="L18">
         <v>10</v>
@@ -76386,7 +76568,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D19" t="s">
         <v>447</v>
@@ -76407,7 +76589,7 @@
         <v>412</v>
       </c>
       <c r="K19" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
       <c r="L19">
         <v>10</v>
@@ -76424,7 +76606,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D20" t="s">
         <v>447</v>
@@ -76445,7 +76627,7 @@
         <v>412</v>
       </c>
       <c r="K20" t="s">
-        <v>4699</v>
+        <v>4697</v>
       </c>
       <c r="L20">
         <v>10</v>
@@ -76462,7 +76644,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D21" t="s">
         <v>447</v>
@@ -76483,7 +76665,7 @@
         <v>412</v>
       </c>
       <c r="K21" t="s">
-        <v>4695</v>
+        <v>4698</v>
       </c>
       <c r="L21">
         <v>10</v>
@@ -76500,7 +76682,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D22" t="s">
         <v>447</v>
@@ -76521,7 +76703,7 @@
         <v>412</v>
       </c>
       <c r="K22" t="s">
-        <v>4697</v>
+        <v>4700</v>
       </c>
       <c r="L22">
         <v>10</v>
@@ -76538,34 +76720,31 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>453</v>
+        <v>3299</v>
       </c>
       <c r="D23" t="s">
-        <v>447</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>412</v>
+        <v>3296</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2307</v>
+      </c>
+      <c r="G23" t="s">
+        <v>3297</v>
+      </c>
+      <c r="H23" t="s">
+        <v>515</v>
+      </c>
+      <c r="I23" t="s">
+        <v>3298</v>
       </c>
       <c r="K23" t="s">
-        <v>4698</v>
-      </c>
-      <c r="L23">
-        <v>10</v>
+        <v>4702</v>
       </c>
       <c r="M23" t="s">
-        <v>4686</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -76576,34 +76755,31 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>455</v>
+        <v>3300</v>
       </c>
       <c r="D24" t="s">
-        <v>447</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>412</v>
+        <v>3296</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4145</v>
+      </c>
+      <c r="H24" t="s">
+        <v>515</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1537</v>
       </c>
       <c r="K24" t="s">
-        <v>4700</v>
-      </c>
-      <c r="L24">
-        <v>10</v>
+        <v>4703</v>
       </c>
       <c r="M24" t="s">
-        <v>4686</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -76614,28 +76790,22 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>3299</v>
+        <v>2555</v>
       </c>
       <c r="D25" t="s">
-        <v>3296</v>
+        <v>2556</v>
       </c>
       <c r="E25" t="s">
-        <v>2307</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>2307</v>
-      </c>
-      <c r="G25" t="s">
-        <v>3297</v>
+        <v>3</v>
       </c>
       <c r="H25" t="s">
         <v>515</v>
       </c>
-      <c r="I25" t="s">
-        <v>3298</v>
-      </c>
       <c r="K25" t="s">
-        <v>4702</v>
+        <v>4705</v>
       </c>
       <c r="M25" t="s">
         <v>4704</v>
@@ -76649,28 +76819,22 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>3300</v>
+        <v>2557</v>
       </c>
       <c r="D26" t="s">
-        <v>3296</v>
+        <v>2556</v>
       </c>
       <c r="E26" t="s">
-        <v>2307</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" t="s">
-        <v>4145</v>
+        <v>3</v>
       </c>
       <c r="H26" t="s">
         <v>515</v>
       </c>
-      <c r="I26" t="s">
-        <v>1537</v>
-      </c>
       <c r="K26" t="s">
-        <v>4703</v>
+        <v>4706</v>
       </c>
       <c r="M26" t="s">
         <v>4704</v>
@@ -76684,7 +76848,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>2555</v>
+        <v>2558</v>
       </c>
       <c r="D27" t="s">
         <v>2556</v>
@@ -76699,7 +76863,7 @@
         <v>515</v>
       </c>
       <c r="K27" t="s">
-        <v>4705</v>
+        <v>4707</v>
       </c>
       <c r="M27" t="s">
         <v>4704</v>
@@ -76713,22 +76877,25 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>2557</v>
+        <v>1130</v>
       </c>
       <c r="D28" t="s">
-        <v>2556</v>
+        <v>1131</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
+        <v>4145</v>
       </c>
       <c r="H28" t="s">
         <v>515</v>
       </c>
+      <c r="I28" t="s">
+        <v>180</v>
+      </c>
       <c r="K28" t="s">
-        <v>4706</v>
+        <v>4711</v>
       </c>
       <c r="M28" t="s">
         <v>4704</v>
@@ -76742,22 +76909,25 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>2558</v>
+        <v>1133</v>
       </c>
       <c r="D29" t="s">
-        <v>2556</v>
+        <v>1131</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>4145</v>
       </c>
       <c r="H29" t="s">
         <v>515</v>
       </c>
+      <c r="I29" t="s">
+        <v>180</v>
+      </c>
       <c r="K29" t="s">
-        <v>4707</v>
+        <v>4712</v>
       </c>
       <c r="M29" t="s">
         <v>4704</v>
@@ -76771,7 +76941,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>1130</v>
+        <v>1134</v>
       </c>
       <c r="D30" t="s">
         <v>1131</v>
@@ -76789,7 +76959,7 @@
         <v>180</v>
       </c>
       <c r="K30" t="s">
-        <v>4711</v>
+        <v>4713</v>
       </c>
       <c r="M30" t="s">
         <v>4704</v>
@@ -76803,7 +76973,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="D31" t="s">
         <v>1131</v>
@@ -76821,7 +76991,7 @@
         <v>180</v>
       </c>
       <c r="K31" t="s">
-        <v>4712</v>
+        <v>4714</v>
       </c>
       <c r="M31" t="s">
         <v>4704</v>
@@ -76829,19 +76999,19 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4599</v>
+        <v>4708</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>1134</v>
+        <v>2689</v>
       </c>
       <c r="D32" t="s">
-        <v>1131</v>
+        <v>2690</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F32" t="s">
         <v>4145</v>
@@ -76849,11 +77019,11 @@
       <c r="H32" t="s">
         <v>515</v>
       </c>
-      <c r="I32" t="s">
-        <v>180</v>
+      <c r="I32">
+        <v>53260</v>
       </c>
       <c r="K32" t="s">
-        <v>4713</v>
+        <v>4736</v>
       </c>
       <c r="M32" t="s">
         <v>4704</v>
@@ -76861,19 +77031,19 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4599</v>
+        <v>4708</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>1135</v>
+        <v>2691</v>
       </c>
       <c r="D33" t="s">
-        <v>1131</v>
+        <v>2690</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F33" t="s">
         <v>4145</v>
@@ -76881,11 +77051,11 @@
       <c r="H33" t="s">
         <v>515</v>
       </c>
-      <c r="I33" t="s">
-        <v>180</v>
+      <c r="I33">
+        <v>53260</v>
       </c>
       <c r="K33" t="s">
-        <v>4714</v>
+        <v>4737</v>
       </c>
       <c r="M33" t="s">
         <v>4704</v>
@@ -76899,7 +77069,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>2689</v>
+        <v>2692</v>
       </c>
       <c r="D34" t="s">
         <v>2690</v>
@@ -76917,7 +77087,7 @@
         <v>53260</v>
       </c>
       <c r="K34" t="s">
-        <v>4736</v>
+        <v>4738</v>
       </c>
       <c r="M34" t="s">
         <v>4704</v>
@@ -76931,10 +77101,10 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>2691</v>
+        <v>2675</v>
       </c>
       <c r="D35" t="s">
-        <v>2690</v>
+        <v>2676</v>
       </c>
       <c r="E35" t="s">
         <v>2615</v>
@@ -76945,11 +77115,11 @@
       <c r="H35" t="s">
         <v>515</v>
       </c>
-      <c r="I35">
-        <v>53260</v>
+      <c r="I35" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K35" t="s">
-        <v>4737</v>
+        <v>4740</v>
       </c>
       <c r="M35" t="s">
         <v>4704</v>
@@ -76963,10 +77133,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>2692</v>
+        <v>2677</v>
       </c>
       <c r="D36" t="s">
-        <v>2690</v>
+        <v>2676</v>
       </c>
       <c r="E36" t="s">
         <v>2615</v>
@@ -76977,11 +77147,11 @@
       <c r="H36" t="s">
         <v>515</v>
       </c>
-      <c r="I36">
-        <v>53260</v>
+      <c r="I36" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K36" t="s">
-        <v>4738</v>
+        <v>4741</v>
       </c>
       <c r="M36" t="s">
         <v>4704</v>
@@ -76995,7 +77165,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>2675</v>
+        <v>2678</v>
       </c>
       <c r="D37" t="s">
         <v>2676</v>
@@ -77013,7 +77183,7 @@
         <v>2591</v>
       </c>
       <c r="K37" t="s">
-        <v>4740</v>
+        <v>4742</v>
       </c>
       <c r="M37" t="s">
         <v>4704</v>
@@ -77027,7 +77197,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>2677</v>
+        <v>2679</v>
       </c>
       <c r="D38" t="s">
         <v>2676</v>
@@ -77045,7 +77215,7 @@
         <v>2591</v>
       </c>
       <c r="K38" t="s">
-        <v>4741</v>
+        <v>4743</v>
       </c>
       <c r="M38" t="s">
         <v>4704</v>
@@ -77059,25 +77229,19 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>2678</v>
+        <v>2680</v>
       </c>
       <c r="D39" t="s">
-        <v>2676</v>
+        <v>2681</v>
       </c>
       <c r="E39" t="s">
         <v>2615</v>
       </c>
-      <c r="F39" t="s">
-        <v>4145</v>
-      </c>
       <c r="H39" t="s">
         <v>515</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>2591</v>
-      </c>
       <c r="K39" t="s">
-        <v>4742</v>
+        <v>4739</v>
       </c>
       <c r="M39" t="s">
         <v>4704</v>
@@ -77091,10 +77255,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>2679</v>
+        <v>2693</v>
       </c>
       <c r="D40" t="s">
-        <v>2676</v>
+        <v>2694</v>
       </c>
       <c r="E40" t="s">
         <v>2615</v>
@@ -77105,11 +77269,11 @@
       <c r="H40" t="s">
         <v>515</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>2591</v>
+      <c r="I40">
+        <v>53260</v>
       </c>
       <c r="K40" t="s">
-        <v>4743</v>
+        <v>4744</v>
       </c>
       <c r="M40" t="s">
         <v>4704</v>
@@ -77123,19 +77287,25 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>2680</v>
+        <v>2696</v>
       </c>
       <c r="D41" t="s">
-        <v>2681</v>
+        <v>2694</v>
       </c>
       <c r="E41" t="s">
         <v>2615</v>
       </c>
+      <c r="F41" t="s">
+        <v>4145</v>
+      </c>
       <c r="H41" t="s">
         <v>515</v>
       </c>
+      <c r="I41">
+        <v>53260</v>
+      </c>
       <c r="K41" t="s">
-        <v>4739</v>
+        <v>4745</v>
       </c>
       <c r="M41" t="s">
         <v>4704</v>
@@ -77149,7 +77319,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>2693</v>
+        <v>2697</v>
       </c>
       <c r="D42" t="s">
         <v>2694</v>
@@ -77167,7 +77337,7 @@
         <v>53260</v>
       </c>
       <c r="K42" t="s">
-        <v>4744</v>
+        <v>4746</v>
       </c>
       <c r="M42" t="s">
         <v>4704</v>
@@ -77181,10 +77351,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>2696</v>
+        <v>2658</v>
       </c>
       <c r="D43" t="s">
-        <v>2694</v>
+        <v>2659</v>
       </c>
       <c r="E43" t="s">
         <v>2615</v>
@@ -77192,14 +77362,14 @@
       <c r="F43" t="s">
         <v>4145</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="I43">
-        <v>53260</v>
+      <c r="I43" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K43" t="s">
-        <v>4745</v>
+        <v>4747</v>
       </c>
       <c r="M43" t="s">
         <v>4704</v>
@@ -77213,10 +77383,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>2697</v>
+        <v>2661</v>
       </c>
       <c r="D44" t="s">
-        <v>2694</v>
+        <v>2659</v>
       </c>
       <c r="E44" t="s">
         <v>2615</v>
@@ -77224,14 +77394,14 @@
       <c r="F44" t="s">
         <v>4145</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="I44">
-        <v>53260</v>
+      <c r="I44" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K44" t="s">
-        <v>4746</v>
+        <v>4748</v>
       </c>
       <c r="M44" t="s">
         <v>4704</v>
@@ -77245,7 +77415,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>2658</v>
+        <v>2662</v>
       </c>
       <c r="D45" t="s">
         <v>2659</v>
@@ -77263,7 +77433,7 @@
         <v>2591</v>
       </c>
       <c r="K45" t="s">
-        <v>4747</v>
+        <v>4749</v>
       </c>
       <c r="M45" t="s">
         <v>4704</v>
@@ -77271,31 +77441,31 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4708</v>
+        <v>4751</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>2661</v>
+        <v>1142</v>
       </c>
       <c r="D46" t="s">
-        <v>2659</v>
+        <v>1137</v>
       </c>
       <c r="E46" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F46" t="s">
         <v>4145</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" t="s">
         <v>515</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>2591</v>
+      <c r="I46" t="s">
+        <v>180</v>
       </c>
       <c r="K46" t="s">
-        <v>4748</v>
+        <v>4756</v>
       </c>
       <c r="M46" t="s">
         <v>4704</v>
@@ -77303,31 +77473,31 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4708</v>
+        <v>4751</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>2662</v>
+        <v>1143</v>
       </c>
       <c r="D47" t="s">
-        <v>2659</v>
+        <v>1137</v>
       </c>
       <c r="E47" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F47" t="s">
         <v>4145</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" t="s">
         <v>515</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>2591</v>
+      <c r="I47" t="s">
+        <v>180</v>
       </c>
       <c r="K47" t="s">
-        <v>4749</v>
+        <v>4757</v>
       </c>
       <c r="M47" t="s">
         <v>4704</v>
@@ -77341,7 +77511,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="D48" t="s">
         <v>1137</v>
@@ -77359,7 +77529,7 @@
         <v>180</v>
       </c>
       <c r="K48" t="s">
-        <v>4756</v>
+        <v>4758</v>
       </c>
       <c r="M48" t="s">
         <v>4704</v>
@@ -77373,7 +77543,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="D49" t="s">
         <v>1137</v>
@@ -77391,7 +77561,7 @@
         <v>180</v>
       </c>
       <c r="K49" t="s">
-        <v>4757</v>
+        <v>4759</v>
       </c>
       <c r="M49" t="s">
         <v>4704</v>
@@ -77405,7 +77575,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="D50" t="s">
         <v>1137</v>
@@ -77423,7 +77593,7 @@
         <v>180</v>
       </c>
       <c r="K50" t="s">
-        <v>4758</v>
+        <v>4760</v>
       </c>
       <c r="M50" t="s">
         <v>4704</v>
@@ -77437,7 +77607,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>1145</v>
+        <v>1151</v>
       </c>
       <c r="D51" t="s">
         <v>1137</v>
@@ -77455,7 +77625,7 @@
         <v>180</v>
       </c>
       <c r="K51" t="s">
-        <v>4759</v>
+        <v>4761</v>
       </c>
       <c r="M51" t="s">
         <v>4704</v>
@@ -77469,7 +77639,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>1146</v>
+        <v>1152</v>
       </c>
       <c r="D52" t="s">
         <v>1137</v>
@@ -77487,7 +77657,7 @@
         <v>180</v>
       </c>
       <c r="K52" t="s">
-        <v>4760</v>
+        <v>4762</v>
       </c>
       <c r="M52" t="s">
         <v>4704</v>
@@ -77501,7 +77671,7 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>1151</v>
+        <v>1159</v>
       </c>
       <c r="D53" t="s">
         <v>1137</v>
@@ -77519,78 +77689,15 @@
         <v>180</v>
       </c>
       <c r="K53" t="s">
-        <v>4761</v>
+        <v>4763</v>
       </c>
       <c r="M53" t="s">
         <v>4704</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B54">
-        <v>53</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D54" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E54" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F54" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H54" t="s">
-        <v>515</v>
-      </c>
-      <c r="I54" t="s">
-        <v>180</v>
-      </c>
-      <c r="K54" t="s">
-        <v>4762</v>
-      </c>
-      <c r="M54" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B55">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D55" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E55" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F55" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H55" t="s">
-        <v>515</v>
-      </c>
-      <c r="I55" t="s">
-        <v>180</v>
-      </c>
-      <c r="K55" t="s">
-        <v>4763</v>
-      </c>
-      <c r="M55" t="s">
-        <v>4704</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -78272,10 +78379,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78957,204 +79064,59 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1997</v>
+        <v>3698</v>
       </c>
       <c r="D22" t="s">
-        <v>1998</v>
+        <v>3696</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
       <c r="H22" t="s">
-        <v>412</v>
+        <v>186</v>
       </c>
       <c r="K22" t="s">
-        <v>4608</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
+        <v>3144</v>
       </c>
       <c r="M22" t="s">
-        <v>4686</v>
+        <v>4685</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4599</v>
+        <v>4751</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>1999</v>
+        <v>3528</v>
       </c>
       <c r="D23" t="s">
-        <v>1998</v>
+        <v>3526</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>1138</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4145</v>
       </c>
       <c r="H23" t="s">
-        <v>412</v>
+        <v>348</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1537</v>
       </c>
       <c r="K23" t="s">
-        <v>4609</v>
-      </c>
-      <c r="L23">
-        <v>10</v>
+        <v>4752</v>
       </c>
       <c r="M23" t="s">
-        <v>4686</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>4599</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" t="s">
-        <v>412</v>
-      </c>
-      <c r="K24" t="s">
-        <v>2001</v>
-      </c>
-      <c r="L24">
-        <v>10</v>
-      </c>
-      <c r="M24" t="s">
-        <v>4686</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>4599</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2002</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" t="s">
-        <v>412</v>
-      </c>
-      <c r="K25" t="s">
-        <v>4610</v>
-      </c>
-      <c r="L25">
-        <v>10</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4686</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4599</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2003</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" t="s">
-        <v>412</v>
-      </c>
-      <c r="K26" t="s">
-        <v>4611</v>
-      </c>
-      <c r="L26">
-        <v>10</v>
-      </c>
-      <c r="M26" t="s">
-        <v>4686</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>4599</v>
-      </c>
-      <c r="B27">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3698</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3696</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" t="s">
-        <v>186</v>
-      </c>
-      <c r="K27" t="s">
-        <v>3144</v>
-      </c>
-      <c r="M27" t="s">
-        <v>4685</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3528</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3526</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G28" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H28" t="s">
-        <v>348</v>
-      </c>
-      <c r="I28" t="s">
-        <v>1537</v>
-      </c>
-      <c r="K28" t="s">
-        <v>4752</v>
-      </c>
-      <c r="M28" t="s">
         <v>4753</v>
       </c>
     </row>

</xml_diff>

<commit_message>
galaga driver promoted to fully working status
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17556" uniqueCount="4786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17549" uniqueCount="4785">
   <si>
     <t>TODO</t>
   </si>
@@ -14109,9 +14109,6 @@
   </si>
   <si>
     <t>sound partially works</t>
-  </si>
-  <si>
-    <t>no samples support</t>
   </si>
   <si>
     <t>Blue Print (Midway)</t>
@@ -15268,7 +15265,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -63710,10 +63707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M461"/>
+  <dimension ref="A1:M468"/>
   <sheetViews>
-    <sheetView topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="M453" sqref="M453"/>
+    <sheetView topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="B457" sqref="B457:B468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75040,7 +75037,7 @@
         <v>186</v>
       </c>
       <c r="L427" t="s">
-        <v>4687</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="428" spans="1:12" x14ac:dyDescent="0.25">
@@ -75066,7 +75063,7 @@
         <v>186</v>
       </c>
       <c r="L428" t="s">
-        <v>4688</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="429" spans="1:12" x14ac:dyDescent="0.25">
@@ -75095,7 +75092,7 @@
         <v>180</v>
       </c>
       <c r="L429" t="s">
-        <v>4689</v>
+        <v>4688</v>
       </c>
     </row>
     <row r="430" spans="1:12" x14ac:dyDescent="0.25">
@@ -75124,7 +75121,7 @@
         <v>180</v>
       </c>
       <c r="L430" t="s">
-        <v>4690</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="431" spans="1:12" x14ac:dyDescent="0.25">
@@ -75153,7 +75150,7 @@
         <v>1306</v>
       </c>
       <c r="L431" t="s">
-        <v>4691</v>
+        <v>4690</v>
       </c>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.25">
@@ -75182,7 +75179,7 @@
         <v>1306</v>
       </c>
       <c r="L432" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.25">
@@ -75234,12 +75231,12 @@
         <v>186</v>
       </c>
       <c r="L434" t="s">
-        <v>4693</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="435" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B435">
         <v>434</v>
@@ -75260,12 +75257,12 @@
         <v>1885</v>
       </c>
       <c r="L435" t="s">
-        <v>4715</v>
+        <v>4714</v>
       </c>
     </row>
     <row r="436" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B436">
         <v>435</v>
@@ -75286,12 +75283,12 @@
         <v>1885</v>
       </c>
       <c r="L436" t="s">
-        <v>4716</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="437" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B437">
         <v>436</v>
@@ -75312,12 +75309,12 @@
         <v>1885</v>
       </c>
       <c r="L437" t="s">
-        <v>4717</v>
+        <v>4716</v>
       </c>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B438">
         <v>437</v>
@@ -75338,12 +75335,12 @@
         <v>1885</v>
       </c>
       <c r="L438" t="s">
-        <v>4718</v>
+        <v>4717</v>
       </c>
     </row>
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B439">
         <v>438</v>
@@ -75364,12 +75361,12 @@
         <v>1885</v>
       </c>
       <c r="L439" t="s">
-        <v>4719</v>
+        <v>4718</v>
       </c>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B440">
         <v>439</v>
@@ -75390,12 +75387,12 @@
         <v>1885</v>
       </c>
       <c r="L440" t="s">
-        <v>4720</v>
+        <v>4719</v>
       </c>
     </row>
     <row r="441" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B441">
         <v>440</v>
@@ -75416,12 +75413,12 @@
         <v>1885</v>
       </c>
       <c r="L441" t="s">
-        <v>4721</v>
+        <v>4720</v>
       </c>
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B442">
         <v>441</v>
@@ -75442,12 +75439,12 @@
         <v>1885</v>
       </c>
       <c r="L442" t="s">
-        <v>4722</v>
+        <v>4721</v>
       </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B443">
         <v>442</v>
@@ -75468,12 +75465,12 @@
         <v>1885</v>
       </c>
       <c r="L443" t="s">
-        <v>4723</v>
+        <v>4722</v>
       </c>
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B444">
         <v>443</v>
@@ -75494,12 +75491,12 @@
         <v>1885</v>
       </c>
       <c r="L444" t="s">
-        <v>4724</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="445" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B445">
         <v>444</v>
@@ -75520,12 +75517,12 @@
         <v>1885</v>
       </c>
       <c r="L445" t="s">
-        <v>4725</v>
+        <v>4724</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B446">
         <v>445</v>
@@ -75549,12 +75546,12 @@
         <v>53260</v>
       </c>
       <c r="L446" t="s">
-        <v>4754</v>
+        <v>4753</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B447">
         <v>446</v>
@@ -75578,12 +75575,12 @@
         <v>53260</v>
       </c>
       <c r="L447" t="s">
-        <v>4755</v>
+        <v>4754</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B448">
         <v>447</v>
@@ -75615,7 +75612,7 @@
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B449">
         <v>448</v>
@@ -75642,12 +75639,12 @@
         <v>1537</v>
       </c>
       <c r="L449" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B450">
         <v>449</v>
@@ -75668,12 +75665,12 @@
         <v>348</v>
       </c>
       <c r="L450" t="s">
-        <v>4781</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B451">
         <v>450</v>
@@ -75694,12 +75691,12 @@
         <v>348</v>
       </c>
       <c r="L451" t="s">
-        <v>4782</v>
+        <v>4781</v>
       </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B452">
         <v>451</v>
@@ -75720,12 +75717,12 @@
         <v>348</v>
       </c>
       <c r="L452" t="s">
-        <v>4783</v>
+        <v>4782</v>
       </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B453">
         <v>452</v>
@@ -75746,12 +75743,12 @@
         <v>348</v>
       </c>
       <c r="L453" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B454">
         <v>453</v>
@@ -75769,12 +75766,12 @@
         <v>1537</v>
       </c>
       <c r="L454" t="s">
-        <v>4780</v>
+        <v>4779</v>
       </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B455">
         <v>454</v>
@@ -75797,7 +75794,7 @@
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B456">
         <v>455</v>
@@ -75820,7 +75817,7 @@
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B457">
         <v>456</v>
@@ -75843,7 +75840,7 @@
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B458">
         <v>457</v>
@@ -75866,7 +75863,7 @@
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B459">
         <v>458</v>
@@ -75889,7 +75886,7 @@
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B460">
         <v>459</v>
@@ -75918,7 +75915,7 @@
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="B461">
         <v>460</v>
@@ -75943,6 +75940,230 @@
       </c>
       <c r="L461" t="s">
         <v>4537</v>
+      </c>
+    </row>
+    <row r="462" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>4750</v>
+      </c>
+      <c r="B462">
+        <v>461</v>
+      </c>
+      <c r="C462" t="s">
+        <v>446</v>
+      </c>
+      <c r="D462" t="s">
+        <v>447</v>
+      </c>
+      <c r="E462" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F462" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G462" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I462" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J462" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L462" t="s">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="463" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B463">
+        <v>462</v>
+      </c>
+      <c r="C463" t="s">
+        <v>449</v>
+      </c>
+      <c r="D463" t="s">
+        <v>447</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F463" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G463" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I463" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J463" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L463" t="s">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="464" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B464">
+        <v>463</v>
+      </c>
+      <c r="C464" t="s">
+        <v>450</v>
+      </c>
+      <c r="D464" t="s">
+        <v>447</v>
+      </c>
+      <c r="E464" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F464" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G464" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I464" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J464" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L464" t="s">
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="465" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B465">
+        <v>464</v>
+      </c>
+      <c r="C465" t="s">
+        <v>451</v>
+      </c>
+      <c r="D465" t="s">
+        <v>447</v>
+      </c>
+      <c r="E465" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F465" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G465" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I465" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J465" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L465" t="s">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="466" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B466">
+        <v>465</v>
+      </c>
+      <c r="C466" t="s">
+        <v>452</v>
+      </c>
+      <c r="D466" t="s">
+        <v>447</v>
+      </c>
+      <c r="E466" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F466" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G466" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I466" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J466" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L466" t="s">
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B467">
+        <v>466</v>
+      </c>
+      <c r="C467" t="s">
+        <v>453</v>
+      </c>
+      <c r="D467" t="s">
+        <v>447</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F467" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G467" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I467" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J467" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L467" t="s">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="468" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>4784</v>
+      </c>
+      <c r="B468">
+        <v>467</v>
+      </c>
+      <c r="C468" t="s">
+        <v>455</v>
+      </c>
+      <c r="D468" t="s">
+        <v>447</v>
+      </c>
+      <c r="E468" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F468" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G468" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I468" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J468" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L468" t="s">
+        <v>4699</v>
       </c>
     </row>
   </sheetData>
@@ -75953,10 +76174,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76454,34 +76675,31 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>446</v>
+        <v>3299</v>
       </c>
       <c r="D16" t="s">
-        <v>447</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>412</v>
+        <v>3296</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2307</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3297</v>
+      </c>
+      <c r="H16" t="s">
+        <v>515</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3298</v>
       </c>
       <c r="K16" t="s">
-        <v>4694</v>
-      </c>
-      <c r="L16">
-        <v>10</v>
+        <v>4701</v>
       </c>
       <c r="M16" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -76492,34 +76710,31 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>449</v>
+        <v>3300</v>
       </c>
       <c r="D17" t="s">
-        <v>447</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>412</v>
+        <v>3296</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4145</v>
+      </c>
+      <c r="H17" t="s">
+        <v>515</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1537</v>
       </c>
       <c r="K17" t="s">
-        <v>4696</v>
-      </c>
-      <c r="L17">
-        <v>10</v>
+        <v>4702</v>
       </c>
       <c r="M17" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -76530,34 +76745,25 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>450</v>
+        <v>2555</v>
       </c>
       <c r="D18" t="s">
-        <v>447</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>412</v>
+        <v>2556</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>515</v>
       </c>
       <c r="K18" t="s">
-        <v>4699</v>
-      </c>
-      <c r="L18">
-        <v>10</v>
+        <v>4704</v>
       </c>
       <c r="M18" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -76568,34 +76774,25 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>451</v>
+        <v>2557</v>
       </c>
       <c r="D19" t="s">
-        <v>447</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>412</v>
+        <v>2556</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>515</v>
       </c>
       <c r="K19" t="s">
-        <v>4695</v>
-      </c>
-      <c r="L19">
-        <v>10</v>
+        <v>4705</v>
       </c>
       <c r="M19" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -76606,34 +76803,25 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>452</v>
+        <v>2558</v>
       </c>
       <c r="D20" t="s">
-        <v>447</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>412</v>
+        <v>2556</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>515</v>
       </c>
       <c r="K20" t="s">
-        <v>4697</v>
-      </c>
-      <c r="L20">
-        <v>10</v>
+        <v>4706</v>
       </c>
       <c r="M20" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -76644,34 +76832,28 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>453</v>
+        <v>1130</v>
       </c>
       <c r="D21" t="s">
-        <v>447</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>412</v>
+        <v>1131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4145</v>
+      </c>
+      <c r="H21" t="s">
+        <v>515</v>
+      </c>
+      <c r="I21" t="s">
+        <v>180</v>
       </c>
       <c r="K21" t="s">
-        <v>4698</v>
-      </c>
-      <c r="L21">
-        <v>10</v>
+        <v>4710</v>
       </c>
       <c r="M21" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -76682,34 +76864,28 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>455</v>
+        <v>1133</v>
       </c>
       <c r="D22" t="s">
-        <v>447</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>412</v>
+        <v>1131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4145</v>
+      </c>
+      <c r="H22" t="s">
+        <v>515</v>
+      </c>
+      <c r="I22" t="s">
+        <v>180</v>
       </c>
       <c r="K22" t="s">
-        <v>4700</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
+        <v>4711</v>
       </c>
       <c r="M22" t="s">
-        <v>4686</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -76720,31 +76896,28 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>3299</v>
+        <v>1134</v>
       </c>
       <c r="D23" t="s">
-        <v>3296</v>
+        <v>1131</v>
       </c>
       <c r="E23" t="s">
-        <v>2307</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>2307</v>
-      </c>
-      <c r="G23" t="s">
-        <v>3297</v>
+        <v>4145</v>
       </c>
       <c r="H23" t="s">
         <v>515</v>
       </c>
       <c r="I23" t="s">
-        <v>3298</v>
+        <v>180</v>
       </c>
       <c r="K23" t="s">
-        <v>4702</v>
+        <v>4712</v>
       </c>
       <c r="M23" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -76755,135 +76928,141 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>3300</v>
+        <v>1135</v>
       </c>
       <c r="D24" t="s">
-        <v>3296</v>
+        <v>1131</v>
       </c>
       <c r="E24" t="s">
-        <v>2307</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
         <v>4145</v>
       </c>
       <c r="H24" t="s">
         <v>515</v>
       </c>
       <c r="I24" t="s">
-        <v>1537</v>
+        <v>180</v>
       </c>
       <c r="K24" t="s">
+        <v>4713</v>
+      </c>
+      <c r="M24" t="s">
         <v>4703</v>
-      </c>
-      <c r="M24" t="s">
-        <v>4704</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>2555</v>
+        <v>2689</v>
       </c>
       <c r="D25" t="s">
-        <v>2556</v>
+        <v>2690</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>2615</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>4145</v>
       </c>
       <c r="H25" t="s">
         <v>515</v>
       </c>
+      <c r="I25">
+        <v>53260</v>
+      </c>
       <c r="K25" t="s">
-        <v>4705</v>
+        <v>4735</v>
       </c>
       <c r="M25" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>2557</v>
+        <v>2691</v>
       </c>
       <c r="D26" t="s">
-        <v>2556</v>
+        <v>2690</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>2615</v>
       </c>
       <c r="F26" t="s">
-        <v>3</v>
+        <v>4145</v>
       </c>
       <c r="H26" t="s">
         <v>515</v>
       </c>
+      <c r="I26">
+        <v>53260</v>
+      </c>
       <c r="K26" t="s">
-        <v>4706</v>
+        <v>4736</v>
       </c>
       <c r="M26" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>2558</v>
+        <v>2692</v>
       </c>
       <c r="D27" t="s">
-        <v>2556</v>
+        <v>2690</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>2615</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>4145</v>
       </c>
       <c r="H27" t="s">
         <v>515</v>
       </c>
+      <c r="I27">
+        <v>53260</v>
+      </c>
       <c r="K27" t="s">
-        <v>4707</v>
+        <v>4737</v>
       </c>
       <c r="M27" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>1130</v>
+        <v>2675</v>
       </c>
       <c r="D28" t="s">
-        <v>1131</v>
+        <v>2676</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F28" t="s">
         <v>4145</v>
@@ -76891,31 +77070,31 @@
       <c r="H28" t="s">
         <v>515</v>
       </c>
-      <c r="I28" t="s">
-        <v>180</v>
+      <c r="I28" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K28" t="s">
-        <v>4711</v>
+        <v>4739</v>
       </c>
       <c r="M28" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>1133</v>
+        <v>2677</v>
       </c>
       <c r="D29" t="s">
-        <v>1131</v>
+        <v>2676</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F29" t="s">
         <v>4145</v>
@@ -76923,31 +77102,31 @@
       <c r="H29" t="s">
         <v>515</v>
       </c>
-      <c r="I29" t="s">
-        <v>180</v>
+      <c r="I29" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K29" t="s">
-        <v>4712</v>
+        <v>4740</v>
       </c>
       <c r="M29" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>1134</v>
+        <v>2678</v>
       </c>
       <c r="D30" t="s">
-        <v>1131</v>
+        <v>2676</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F30" t="s">
         <v>4145</v>
@@ -76955,31 +77134,31 @@
       <c r="H30" t="s">
         <v>515</v>
       </c>
-      <c r="I30" t="s">
-        <v>180</v>
+      <c r="I30" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K30" t="s">
-        <v>4713</v>
+        <v>4741</v>
       </c>
       <c r="M30" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4599</v>
+        <v>4707</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>1135</v>
+        <v>2679</v>
       </c>
       <c r="D31" t="s">
-        <v>1131</v>
+        <v>2676</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>2615</v>
       </c>
       <c r="F31" t="s">
         <v>4145</v>
@@ -76987,60 +77166,54 @@
       <c r="H31" t="s">
         <v>515</v>
       </c>
-      <c r="I31" t="s">
-        <v>180</v>
+      <c r="I31" s="1" t="s">
+        <v>2591</v>
       </c>
       <c r="K31" t="s">
-        <v>4714</v>
+        <v>4742</v>
       </c>
       <c r="M31" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>2689</v>
+        <v>2680</v>
       </c>
       <c r="D32" t="s">
-        <v>2690</v>
+        <v>2681</v>
       </c>
       <c r="E32" t="s">
         <v>2615</v>
       </c>
-      <c r="F32" t="s">
-        <v>4145</v>
-      </c>
       <c r="H32" t="s">
         <v>515</v>
       </c>
-      <c r="I32">
-        <v>53260</v>
-      </c>
       <c r="K32" t="s">
-        <v>4736</v>
+        <v>4738</v>
       </c>
       <c r="M32" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>2691</v>
+        <v>2693</v>
       </c>
       <c r="D33" t="s">
-        <v>2690</v>
+        <v>2694</v>
       </c>
       <c r="E33" t="s">
         <v>2615</v>
@@ -77055,24 +77228,24 @@
         <v>53260</v>
       </c>
       <c r="K33" t="s">
-        <v>4737</v>
+        <v>4743</v>
       </c>
       <c r="M33" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>2692</v>
+        <v>2696</v>
       </c>
       <c r="D34" t="s">
-        <v>2690</v>
+        <v>2694</v>
       </c>
       <c r="E34" t="s">
         <v>2615</v>
@@ -77087,24 +77260,24 @@
         <v>53260</v>
       </c>
       <c r="K34" t="s">
-        <v>4738</v>
+        <v>4744</v>
       </c>
       <c r="M34" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>2675</v>
+        <v>2697</v>
       </c>
       <c r="D35" t="s">
-        <v>2676</v>
+        <v>2694</v>
       </c>
       <c r="E35" t="s">
         <v>2615</v>
@@ -77115,28 +77288,28 @@
       <c r="H35" t="s">
         <v>515</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>2591</v>
+      <c r="I35">
+        <v>53260</v>
       </c>
       <c r="K35" t="s">
-        <v>4740</v>
+        <v>4745</v>
       </c>
       <c r="M35" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>2677</v>
+        <v>2658</v>
       </c>
       <c r="D36" t="s">
-        <v>2676</v>
+        <v>2659</v>
       </c>
       <c r="E36" t="s">
         <v>2615</v>
@@ -77144,31 +77317,31 @@
       <c r="F36" t="s">
         <v>4145</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>515</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>2591</v>
       </c>
       <c r="K36" t="s">
-        <v>4741</v>
+        <v>4746</v>
       </c>
       <c r="M36" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>2678</v>
+        <v>2661</v>
       </c>
       <c r="D37" t="s">
-        <v>2676</v>
+        <v>2659</v>
       </c>
       <c r="E37" t="s">
         <v>2615</v>
@@ -77176,31 +77349,31 @@
       <c r="F37" t="s">
         <v>4145</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="1" t="s">
         <v>515</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>2591</v>
       </c>
       <c r="K37" t="s">
-        <v>4742</v>
+        <v>4747</v>
       </c>
       <c r="M37" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>2679</v>
+        <v>2662</v>
       </c>
       <c r="D38" t="s">
-        <v>2676</v>
+        <v>2659</v>
       </c>
       <c r="E38" t="s">
         <v>2615</v>
@@ -77208,60 +77381,66 @@
       <c r="F38" t="s">
         <v>4145</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="1" t="s">
         <v>515</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>2591</v>
       </c>
       <c r="K38" t="s">
-        <v>4743</v>
+        <v>4748</v>
       </c>
       <c r="M38" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>2680</v>
+        <v>1142</v>
       </c>
       <c r="D39" t="s">
-        <v>2681</v>
+        <v>1137</v>
       </c>
       <c r="E39" t="s">
-        <v>2615</v>
+        <v>1138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4145</v>
       </c>
       <c r="H39" t="s">
         <v>515</v>
       </c>
+      <c r="I39" t="s">
+        <v>180</v>
+      </c>
       <c r="K39" t="s">
-        <v>4739</v>
+        <v>4755</v>
       </c>
       <c r="M39" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>2693</v>
+        <v>1143</v>
       </c>
       <c r="D40" t="s">
-        <v>2694</v>
+        <v>1137</v>
       </c>
       <c r="E40" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F40" t="s">
         <v>4145</v>
@@ -77269,31 +77448,31 @@
       <c r="H40" t="s">
         <v>515</v>
       </c>
-      <c r="I40">
-        <v>53260</v>
+      <c r="I40" t="s">
+        <v>180</v>
       </c>
       <c r="K40" t="s">
-        <v>4744</v>
+        <v>4756</v>
       </c>
       <c r="M40" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>2696</v>
+        <v>1144</v>
       </c>
       <c r="D41" t="s">
-        <v>2694</v>
+        <v>1137</v>
       </c>
       <c r="E41" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F41" t="s">
         <v>4145</v>
@@ -77301,31 +77480,31 @@
       <c r="H41" t="s">
         <v>515</v>
       </c>
-      <c r="I41">
-        <v>53260</v>
+      <c r="I41" t="s">
+        <v>180</v>
       </c>
       <c r="K41" t="s">
-        <v>4745</v>
+        <v>4757</v>
       </c>
       <c r="M41" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>2697</v>
+        <v>1145</v>
       </c>
       <c r="D42" t="s">
-        <v>2694</v>
+        <v>1137</v>
       </c>
       <c r="E42" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F42" t="s">
         <v>4145</v>
@@ -77333,121 +77512,121 @@
       <c r="H42" t="s">
         <v>515</v>
       </c>
-      <c r="I42">
-        <v>53260</v>
+      <c r="I42" t="s">
+        <v>180</v>
       </c>
       <c r="K42" t="s">
-        <v>4746</v>
+        <v>4758</v>
       </c>
       <c r="M42" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>2658</v>
+        <v>1146</v>
       </c>
       <c r="D43" t="s">
-        <v>2659</v>
+        <v>1137</v>
       </c>
       <c r="E43" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F43" t="s">
         <v>4145</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" t="s">
         <v>515</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>2591</v>
+      <c r="I43" t="s">
+        <v>180</v>
       </c>
       <c r="K43" t="s">
-        <v>4747</v>
+        <v>4759</v>
       </c>
       <c r="M43" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>2661</v>
+        <v>1151</v>
       </c>
       <c r="D44" t="s">
-        <v>2659</v>
+        <v>1137</v>
       </c>
       <c r="E44" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F44" t="s">
         <v>4145</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" t="s">
         <v>515</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>2591</v>
+      <c r="I44" t="s">
+        <v>180</v>
       </c>
       <c r="K44" t="s">
-        <v>4748</v>
+        <v>4760</v>
       </c>
       <c r="M44" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4708</v>
+        <v>4750</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>2662</v>
+        <v>1152</v>
       </c>
       <c r="D45" t="s">
-        <v>2659</v>
+        <v>1137</v>
       </c>
       <c r="E45" t="s">
-        <v>2615</v>
+        <v>1138</v>
       </c>
       <c r="F45" t="s">
         <v>4145</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" t="s">
         <v>515</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>2591</v>
+      <c r="I45" t="s">
+        <v>180</v>
       </c>
       <c r="K45" t="s">
-        <v>4749</v>
+        <v>4761</v>
       </c>
       <c r="M45" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>1142</v>
+        <v>1159</v>
       </c>
       <c r="D46" t="s">
         <v>1137</v>
@@ -77465,234 +77644,10 @@
         <v>180</v>
       </c>
       <c r="K46" t="s">
-        <v>4756</v>
+        <v>4762</v>
       </c>
       <c r="M46" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E47" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F47" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H47" t="s">
-        <v>515</v>
-      </c>
-      <c r="I47" t="s">
-        <v>180</v>
-      </c>
-      <c r="K47" t="s">
-        <v>4757</v>
-      </c>
-      <c r="M47" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1144</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F48" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H48" t="s">
-        <v>515</v>
-      </c>
-      <c r="I48" t="s">
-        <v>180</v>
-      </c>
-      <c r="K48" t="s">
-        <v>4758</v>
-      </c>
-      <c r="M48" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E49" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F49" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H49" t="s">
-        <v>515</v>
-      </c>
-      <c r="I49" t="s">
-        <v>180</v>
-      </c>
-      <c r="K49" t="s">
-        <v>4759</v>
-      </c>
-      <c r="M49" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B50">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1146</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E50" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F50" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H50" t="s">
-        <v>515</v>
-      </c>
-      <c r="I50" t="s">
-        <v>180</v>
-      </c>
-      <c r="K50" t="s">
-        <v>4760</v>
-      </c>
-      <c r="M50" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B51">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E51" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F51" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H51" t="s">
-        <v>515</v>
-      </c>
-      <c r="I51" t="s">
-        <v>180</v>
-      </c>
-      <c r="K51" t="s">
-        <v>4761</v>
-      </c>
-      <c r="M51" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B52">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E52" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F52" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H52" t="s">
-        <v>515</v>
-      </c>
-      <c r="I52" t="s">
-        <v>180</v>
-      </c>
-      <c r="K52" t="s">
-        <v>4762</v>
-      </c>
-      <c r="M52" t="s">
-        <v>4704</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>4751</v>
-      </c>
-      <c r="B53">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E53" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F53" t="s">
-        <v>4145</v>
-      </c>
-      <c r="H53" t="s">
-        <v>515</v>
-      </c>
-      <c r="I53" t="s">
-        <v>180</v>
-      </c>
-      <c r="K53" t="s">
-        <v>4763</v>
-      </c>
-      <c r="M53" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
     </row>
   </sheetData>
@@ -77805,7 +77760,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -77829,15 +77784,15 @@
         <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
       <c r="L4" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -77861,15 +77816,15 @@
         <v>180</v>
       </c>
       <c r="K5" t="s">
-        <v>4765</v>
+        <v>4764</v>
       </c>
       <c r="L5" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -77893,15 +77848,15 @@
         <v>180</v>
       </c>
       <c r="K6" t="s">
+        <v>4765</v>
+      </c>
+      <c r="L6" t="s">
         <v>4766</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4767</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -77922,15 +77877,15 @@
         <v>515</v>
       </c>
       <c r="K7" t="s">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="L7" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -77951,15 +77906,15 @@
         <v>515</v>
       </c>
       <c r="K8" t="s">
-        <v>4769</v>
+        <v>4768</v>
       </c>
       <c r="L8" t="s">
-        <v>4772</v>
+        <v>4771</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -77980,10 +77935,10 @@
         <v>515</v>
       </c>
       <c r="K9" t="s">
-        <v>4770</v>
+        <v>4769</v>
       </c>
       <c r="L9" t="s">
-        <v>4772</v>
+        <v>4771</v>
       </c>
     </row>
   </sheetData>
@@ -78287,7 +78242,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -78308,7 +78263,7 @@
         <v>1885</v>
       </c>
       <c r="K10" t="s">
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="L10" t="s">
         <v>4384</v>
@@ -78316,7 +78271,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -78337,7 +78292,7 @@
         <v>1885</v>
       </c>
       <c r="K11" t="s">
-        <v>4734</v>
+        <v>4733</v>
       </c>
       <c r="L11" t="s">
         <v>4384</v>
@@ -78345,7 +78300,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -78366,7 +78321,7 @@
         <v>1885</v>
       </c>
       <c r="K12" t="s">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="L12" t="s">
         <v>4384</v>
@@ -79087,7 +79042,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -79114,10 +79069,10 @@
         <v>1537</v>
       </c>
       <c r="K23" t="s">
+        <v>4751</v>
+      </c>
+      <c r="M23" t="s">
         <v>4752</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4753</v>
       </c>
     </row>
   </sheetData>
@@ -80737,15 +80692,15 @@
         <v>515</v>
       </c>
       <c r="L25" t="s">
+        <v>4708</v>
+      </c>
+      <c r="M25" t="s">
         <v>4709</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4710</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -80766,15 +80721,15 @@
         <v>1885</v>
       </c>
       <c r="L26" t="s">
-        <v>4726</v>
+        <v>4725</v>
       </c>
       <c r="M26" t="s">
-        <v>4730</v>
+        <v>4729</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -80795,15 +80750,15 @@
         <v>1885</v>
       </c>
       <c r="L27" t="s">
-        <v>4727</v>
+        <v>4726</v>
       </c>
       <c r="M27" t="s">
-        <v>4731</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -80824,15 +80779,15 @@
         <v>1885</v>
       </c>
       <c r="L28" t="s">
-        <v>4728</v>
+        <v>4727</v>
       </c>
       <c r="M28" t="s">
-        <v>4732</v>
+        <v>4731</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -80853,15 +80808,15 @@
         <v>1885</v>
       </c>
       <c r="L29" t="s">
-        <v>4729</v>
+        <v>4728</v>
       </c>
       <c r="M29" t="s">
-        <v>4732</v>
+        <v>4731</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -80885,15 +80840,15 @@
         <v>180</v>
       </c>
       <c r="L30" t="s">
-        <v>4773</v>
+        <v>4772</v>
       </c>
       <c r="M30" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -80917,15 +80872,15 @@
         <v>180</v>
       </c>
       <c r="L31" t="s">
-        <v>4774</v>
+        <v>4773</v>
       </c>
       <c r="M31" t="s">
-        <v>4778</v>
+        <v>4777</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -80949,15 +80904,15 @@
         <v>180</v>
       </c>
       <c r="L32" t="s">
-        <v>4775</v>
+        <v>4774</v>
       </c>
       <c r="M32" t="s">
-        <v>4779</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -80981,10 +80936,10 @@
         <v>180</v>
       </c>
       <c r="L33" t="s">
-        <v>4776</v>
+        <v>4775</v>
       </c>
       <c r="M33" t="s">
-        <v>4779</v>
+        <v>4778</v>
       </c>
     </row>
   </sheetData>
@@ -81813,7 +81768,7 @@
         <v>3298</v>
       </c>
       <c r="M29" t="s">
-        <v>4701</v>
+        <v>4700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
promoted rallyx driver to fully working game driver
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17549" uniqueCount="4785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17546" uniqueCount="4784">
   <si>
     <t>TODO</t>
   </si>
@@ -13569,9 +13569,6 @@
   </si>
   <si>
     <t>New Rally X</t>
-  </si>
-  <si>
-    <t>no sample support</t>
   </si>
   <si>
     <t>Yie Ar Kung-Fu (set 1)</t>
@@ -15265,21 +15262,21 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="M1" s="4" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -15986,7 +15983,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16013,15 +16010,15 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>4680</v>
+        <v>4679</v>
       </c>
       <c r="N5" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16048,15 +16045,15 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>4681</v>
+        <v>4680</v>
       </c>
       <c r="N6" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16083,15 +16080,15 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>4682</v>
+        <v>4681</v>
       </c>
       <c r="N7" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -16118,10 +16115,10 @@
         <v>180</v>
       </c>
       <c r="M8" t="s">
+        <v>4682</v>
+      </c>
+      <c r="N8" t="s">
         <v>4683</v>
-      </c>
-      <c r="N8" t="s">
-        <v>4684</v>
       </c>
     </row>
   </sheetData>
@@ -63707,10 +63704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M468"/>
+  <dimension ref="A1:M471"/>
   <sheetViews>
-    <sheetView topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="B457" sqref="B457:B468"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="D472" sqref="D472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72490,7 +72487,7 @@
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B336">
         <v>335</v>
@@ -72517,12 +72514,12 @@
         <v>3186</v>
       </c>
       <c r="M336" t="s">
-        <v>4520</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B337">
         <v>336</v>
@@ -72546,15 +72543,15 @@
         <v>328</v>
       </c>
       <c r="L337" t="s">
+        <v>4518</v>
+      </c>
+      <c r="M337" t="s">
         <v>4519</v>
-      </c>
-      <c r="M337" t="s">
-        <v>4520</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B338">
         <v>337</v>
@@ -72575,15 +72572,15 @@
         <v>1310</v>
       </c>
       <c r="L338" t="s">
-        <v>4521</v>
+        <v>4520</v>
       </c>
       <c r="M338" t="s">
-        <v>4524</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B339">
         <v>338</v>
@@ -72604,15 +72601,15 @@
         <v>1310</v>
       </c>
       <c r="L339" t="s">
-        <v>4522</v>
+        <v>4521</v>
       </c>
       <c r="M339" t="s">
-        <v>4524</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B340">
         <v>339</v>
@@ -72633,15 +72630,15 @@
         <v>1310</v>
       </c>
       <c r="L340" t="s">
+        <v>4522</v>
+      </c>
+      <c r="M340" t="s">
         <v>4523</v>
-      </c>
-      <c r="M340" t="s">
-        <v>4524</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B341">
         <v>340</v>
@@ -72667,12 +72664,12 @@
         <v>329</v>
       </c>
       <c r="L341" t="s">
-        <v>4525</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B342">
         <v>341</v>
@@ -72698,12 +72695,12 @@
         <v>329</v>
       </c>
       <c r="L342" t="s">
-        <v>4526</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B343">
         <v>342</v>
@@ -72729,12 +72726,12 @@
         <v>329</v>
       </c>
       <c r="L343" t="s">
-        <v>4527</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B344">
         <v>343</v>
@@ -72760,12 +72757,12 @@
         <v>329</v>
       </c>
       <c r="L344" t="s">
-        <v>4528</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B345">
         <v>344</v>
@@ -72791,12 +72788,12 @@
         <v>329</v>
       </c>
       <c r="L345" t="s">
-        <v>4529</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B346">
         <v>345</v>
@@ -72822,12 +72819,12 @@
         <v>329</v>
       </c>
       <c r="L346" t="s">
-        <v>4530</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B347">
         <v>346</v>
@@ -72853,12 +72850,12 @@
         <v>329</v>
       </c>
       <c r="L347" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B348">
         <v>347</v>
@@ -72882,12 +72879,12 @@
         <v>180</v>
       </c>
       <c r="L348" t="s">
-        <v>4532</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B349">
         <v>348</v>
@@ -72911,12 +72908,12 @@
         <v>180</v>
       </c>
       <c r="L349" t="s">
-        <v>4534</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B350">
         <v>349</v>
@@ -72940,12 +72937,12 @@
         <v>180</v>
       </c>
       <c r="L350" t="s">
-        <v>4533</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B351">
         <v>350</v>
@@ -72969,12 +72966,12 @@
         <v>180</v>
       </c>
       <c r="L351" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B352">
         <v>351</v>
@@ -73001,12 +72998,12 @@
         <v>328</v>
       </c>
       <c r="L352" t="s">
-        <v>4545</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B353">
         <v>352</v>
@@ -73033,12 +73030,12 @@
         <v>328</v>
       </c>
       <c r="L353" t="s">
-        <v>4544</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B354">
         <v>353</v>
@@ -73068,12 +73065,12 @@
         <v>1306</v>
       </c>
       <c r="L354" t="s">
-        <v>4543</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B355">
         <v>354</v>
@@ -73097,12 +73094,12 @@
         <v>87</v>
       </c>
       <c r="L355" t="s">
-        <v>4562</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B356">
         <v>355</v>
@@ -73126,12 +73123,12 @@
         <v>87</v>
       </c>
       <c r="L356" t="s">
-        <v>4563</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B357">
         <v>356</v>
@@ -73155,12 +73152,12 @@
         <v>87</v>
       </c>
       <c r="L357" t="s">
-        <v>4564</v>
+        <v>4563</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B358">
         <v>357</v>
@@ -73184,12 +73181,12 @@
         <v>87</v>
       </c>
       <c r="L358" t="s">
-        <v>4565</v>
+        <v>4564</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B359">
         <v>358</v>
@@ -73213,12 +73210,12 @@
         <v>87</v>
       </c>
       <c r="L359" t="s">
-        <v>4566</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B360">
         <v>359</v>
@@ -73242,12 +73239,12 @@
         <v>87</v>
       </c>
       <c r="L360" t="s">
-        <v>4567</v>
+        <v>4566</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B361">
         <v>360</v>
@@ -73271,12 +73268,12 @@
         <v>87</v>
       </c>
       <c r="L361" t="s">
-        <v>4568</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B362">
         <v>361</v>
@@ -73300,12 +73297,12 @@
         <v>87</v>
       </c>
       <c r="L362" t="s">
-        <v>4569</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B363">
         <v>362</v>
@@ -73329,12 +73326,12 @@
         <v>87</v>
       </c>
       <c r="L363" t="s">
-        <v>4570</v>
+        <v>4569</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B364">
         <v>363</v>
@@ -73358,12 +73355,12 @@
         <v>87</v>
       </c>
       <c r="L364" t="s">
-        <v>4571</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B365">
         <v>364</v>
@@ -73387,12 +73384,12 @@
         <v>87</v>
       </c>
       <c r="L365" t="s">
-        <v>4572</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B366">
         <v>365</v>
@@ -73416,12 +73413,12 @@
         <v>87</v>
       </c>
       <c r="L366" t="s">
-        <v>4573</v>
+        <v>4572</v>
       </c>
     </row>
     <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B367">
         <v>366</v>
@@ -73444,12 +73441,12 @@
         <v>186</v>
       </c>
       <c r="L367" t="s">
-        <v>4574</v>
+        <v>4573</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B368">
         <v>367</v>
@@ -73472,12 +73469,12 @@
         <v>186</v>
       </c>
       <c r="L368" t="s">
-        <v>4575</v>
+        <v>4574</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B369">
         <v>368</v>
@@ -73505,7 +73502,7 @@
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B370">
         <v>369</v>
@@ -73530,12 +73527,12 @@
         <v>3193</v>
       </c>
       <c r="L370" t="s">
-        <v>4588</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B371">
         <v>370</v>
@@ -73560,12 +73557,12 @@
         <v>3193</v>
       </c>
       <c r="L371" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="372" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B372">
         <v>371</v>
@@ -73590,12 +73587,12 @@
         <v>3193</v>
       </c>
       <c r="L372" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="373" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B373">
         <v>372</v>
@@ -73620,12 +73617,12 @@
         <v>3193</v>
       </c>
       <c r="L373" t="s">
-        <v>4591</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B374">
         <v>373</v>
@@ -73650,12 +73647,12 @@
         <v>3193</v>
       </c>
       <c r="L374" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B375">
         <v>374</v>
@@ -73683,12 +73680,12 @@
         <v>3207</v>
       </c>
       <c r="L375" t="s">
-        <v>4593</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="376" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B376">
         <v>375</v>
@@ -73716,12 +73713,12 @@
         <v>3207</v>
       </c>
       <c r="L376" t="s">
-        <v>4594</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B377">
         <v>376</v>
@@ -73748,12 +73745,12 @@
         <v>1306</v>
       </c>
       <c r="L377" t="s">
-        <v>4598</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="378" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B378">
         <v>377</v>
@@ -73774,12 +73771,12 @@
         <v>323</v>
       </c>
       <c r="L378" t="s">
-        <v>4597</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B379">
         <v>378</v>
@@ -73805,7 +73802,7 @@
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B380">
         <v>379</v>
@@ -73823,12 +73820,12 @@
         <v>2874</v>
       </c>
       <c r="L380" t="s">
-        <v>4600</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="381" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B381">
         <v>380</v>
@@ -73846,12 +73843,12 @@
         <v>2874</v>
       </c>
       <c r="L381" t="s">
-        <v>4601</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B382">
         <v>381</v>
@@ -73869,12 +73866,12 @@
         <v>2874</v>
       </c>
       <c r="L382" t="s">
-        <v>4602</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B383">
         <v>382</v>
@@ -73900,7 +73897,7 @@
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B384">
         <v>383</v>
@@ -73926,7 +73923,7 @@
     </row>
     <row r="385" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B385">
         <v>384</v>
@@ -73944,12 +73941,12 @@
         <v>74</v>
       </c>
       <c r="L385" t="s">
-        <v>4603</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B386">
         <v>385</v>
@@ -73967,12 +73964,12 @@
         <v>74</v>
       </c>
       <c r="L386" t="s">
-        <v>4604</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B387">
         <v>386</v>
@@ -73990,12 +73987,12 @@
         <v>74</v>
       </c>
       <c r="L387" t="s">
-        <v>4605</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B388">
         <v>387</v>
@@ -74015,7 +74012,7 @@
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B389">
         <v>388</v>
@@ -74041,7 +74038,7 @@
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B390">
         <v>389</v>
@@ -74067,7 +74064,7 @@
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B391">
         <v>390</v>
@@ -74085,12 +74082,12 @@
         <v>74</v>
       </c>
       <c r="L391" t="s">
-        <v>4614</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B392">
         <v>391</v>
@@ -74113,7 +74110,7 @@
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B393">
         <v>392</v>
@@ -74136,7 +74133,7 @@
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B394">
         <v>393</v>
@@ -74159,7 +74156,7 @@
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B395">
         <v>394</v>
@@ -74177,12 +74174,12 @@
         <v>74</v>
       </c>
       <c r="L395" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B396">
         <v>395</v>
@@ -74200,12 +74197,12 @@
         <v>74</v>
       </c>
       <c r="L396" t="s">
-        <v>4616</v>
+        <v>4615</v>
       </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B397">
         <v>396</v>
@@ -74223,12 +74220,12 @@
         <v>74</v>
       </c>
       <c r="L397" t="s">
-        <v>4617</v>
+        <v>4616</v>
       </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B398">
         <v>397</v>
@@ -74251,7 +74248,7 @@
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B399">
         <v>398</v>
@@ -74269,12 +74266,12 @@
         <v>2878</v>
       </c>
       <c r="L399" t="s">
-        <v>4606</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B400">
         <v>399</v>
@@ -74292,12 +74289,12 @@
         <v>2878</v>
       </c>
       <c r="L400" t="s">
-        <v>4607</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B401">
         <v>400</v>
@@ -74315,12 +74312,12 @@
         <v>2874</v>
       </c>
       <c r="L401" t="s">
-        <v>4634</v>
+        <v>4633</v>
       </c>
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B402">
         <v>401</v>
@@ -74338,12 +74335,12 @@
         <v>2874</v>
       </c>
       <c r="L402" t="s">
-        <v>4635</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B403">
         <v>402</v>
@@ -74361,12 +74358,12 @@
         <v>74</v>
       </c>
       <c r="L403" t="s">
-        <v>4636</v>
+        <v>4635</v>
       </c>
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B404">
         <v>403</v>
@@ -74384,12 +74381,12 @@
         <v>74</v>
       </c>
       <c r="L404" t="s">
-        <v>4637</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B405">
         <v>404</v>
@@ -74407,12 +74404,12 @@
         <v>186</v>
       </c>
       <c r="L405" t="s">
-        <v>4648</v>
+        <v>4647</v>
       </c>
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B406">
         <v>405</v>
@@ -74435,12 +74432,12 @@
         <v>186</v>
       </c>
       <c r="L406" t="s">
-        <v>4649</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B407">
         <v>406</v>
@@ -74463,12 +74460,12 @@
         <v>186</v>
       </c>
       <c r="L407" t="s">
-        <v>4650</v>
+        <v>4649</v>
       </c>
     </row>
     <row r="408" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B408">
         <v>407</v>
@@ -74489,12 +74486,12 @@
         <v>74</v>
       </c>
       <c r="L408" t="s">
-        <v>4651</v>
+        <v>4650</v>
       </c>
     </row>
     <row r="409" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B409">
         <v>408</v>
@@ -74520,7 +74517,7 @@
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B410">
         <v>409</v>
@@ -74541,12 +74538,12 @@
         <v>74</v>
       </c>
       <c r="L410" t="s">
-        <v>4652</v>
+        <v>4651</v>
       </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B411">
         <v>410</v>
@@ -74572,7 +74569,7 @@
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B412">
         <v>411</v>
@@ -74593,12 +74590,12 @@
         <v>74</v>
       </c>
       <c r="L412" t="s">
-        <v>4653</v>
+        <v>4652</v>
       </c>
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B413">
         <v>412</v>
@@ -74628,12 +74625,12 @@
         <v>180</v>
       </c>
       <c r="L413" t="s">
-        <v>4663</v>
+        <v>4662</v>
       </c>
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B414">
         <v>413</v>
@@ -74663,12 +74660,12 @@
         <v>180</v>
       </c>
       <c r="L414" t="s">
-        <v>4664</v>
+        <v>4663</v>
       </c>
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B415">
         <v>414</v>
@@ -74692,12 +74689,12 @@
         <v>180</v>
       </c>
       <c r="L415" t="s">
-        <v>4665</v>
+        <v>4664</v>
       </c>
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B416">
         <v>415</v>
@@ -74721,12 +74718,12 @@
         <v>180</v>
       </c>
       <c r="L416" t="s">
-        <v>4666</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B417">
         <v>416</v>
@@ -74750,12 +74747,12 @@
         <v>180</v>
       </c>
       <c r="L417" t="s">
-        <v>4667</v>
+        <v>4666</v>
       </c>
     </row>
     <row r="418" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B418">
         <v>417</v>
@@ -74779,12 +74776,12 @@
         <v>180</v>
       </c>
       <c r="L418" t="s">
-        <v>4668</v>
+        <v>4667</v>
       </c>
     </row>
     <row r="419" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B419">
         <v>418</v>
@@ -74808,12 +74805,12 @@
         <v>180</v>
       </c>
       <c r="L419" t="s">
-        <v>4669</v>
+        <v>4668</v>
       </c>
     </row>
     <row r="420" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B420">
         <v>419</v>
@@ -74837,12 +74834,12 @@
         <v>180</v>
       </c>
       <c r="L420" t="s">
-        <v>4670</v>
+        <v>4669</v>
       </c>
     </row>
     <row r="421" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B421">
         <v>420</v>
@@ -74866,12 +74863,12 @@
         <v>180</v>
       </c>
       <c r="L421" t="s">
-        <v>4671</v>
+        <v>4670</v>
       </c>
     </row>
     <row r="422" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B422">
         <v>421</v>
@@ -74895,12 +74892,12 @@
         <v>180</v>
       </c>
       <c r="L422" t="s">
-        <v>4673</v>
+        <v>4672</v>
       </c>
     </row>
     <row r="423" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B423">
         <v>422</v>
@@ -74924,12 +74921,12 @@
         <v>180</v>
       </c>
       <c r="L423" t="s">
-        <v>4672</v>
+        <v>4671</v>
       </c>
     </row>
     <row r="424" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B424">
         <v>423</v>
@@ -74953,12 +74950,12 @@
         <v>180</v>
       </c>
       <c r="L424" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
     </row>
     <row r="425" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B425">
         <v>424</v>
@@ -74982,12 +74979,12 @@
         <v>180</v>
       </c>
       <c r="L425" t="s">
-        <v>4675</v>
+        <v>4674</v>
       </c>
     </row>
     <row r="426" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B426">
         <v>425</v>
@@ -75011,12 +75008,12 @@
         <v>180</v>
       </c>
       <c r="L426" t="s">
-        <v>4676</v>
+        <v>4675</v>
       </c>
     </row>
     <row r="427" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B427">
         <v>426</v>
@@ -75037,12 +75034,12 @@
         <v>186</v>
       </c>
       <c r="L427" t="s">
-        <v>4686</v>
+        <v>4685</v>
       </c>
     </row>
     <row r="428" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B428">
         <v>427</v>
@@ -75063,12 +75060,12 @@
         <v>186</v>
       </c>
       <c r="L428" t="s">
-        <v>4687</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="429" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B429">
         <v>428</v>
@@ -75092,12 +75089,12 @@
         <v>180</v>
       </c>
       <c r="L429" t="s">
-        <v>4688</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="430" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B430">
         <v>429</v>
@@ -75121,12 +75118,12 @@
         <v>180</v>
       </c>
       <c r="L430" t="s">
-        <v>4689</v>
+        <v>4688</v>
       </c>
     </row>
     <row r="431" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B431">
         <v>430</v>
@@ -75150,12 +75147,12 @@
         <v>1306</v>
       </c>
       <c r="L431" t="s">
-        <v>4690</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B432">
         <v>431</v>
@@ -75179,12 +75176,12 @@
         <v>1306</v>
       </c>
       <c r="L432" t="s">
-        <v>4691</v>
+        <v>4690</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B433">
         <v>432</v>
@@ -75210,7 +75207,7 @@
     </row>
     <row r="434" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B434">
         <v>433</v>
@@ -75231,12 +75228,12 @@
         <v>186</v>
       </c>
       <c r="L434" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
     </row>
     <row r="435" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B435">
         <v>434</v>
@@ -75257,12 +75254,12 @@
         <v>1885</v>
       </c>
       <c r="L435" t="s">
-        <v>4714</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="436" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B436">
         <v>435</v>
@@ -75283,12 +75280,12 @@
         <v>1885</v>
       </c>
       <c r="L436" t="s">
-        <v>4715</v>
+        <v>4714</v>
       </c>
     </row>
     <row r="437" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B437">
         <v>436</v>
@@ -75309,12 +75306,12 @@
         <v>1885</v>
       </c>
       <c r="L437" t="s">
-        <v>4716</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B438">
         <v>437</v>
@@ -75335,12 +75332,12 @@
         <v>1885</v>
       </c>
       <c r="L438" t="s">
-        <v>4717</v>
+        <v>4716</v>
       </c>
     </row>
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B439">
         <v>438</v>
@@ -75361,12 +75358,12 @@
         <v>1885</v>
       </c>
       <c r="L439" t="s">
-        <v>4718</v>
+        <v>4717</v>
       </c>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B440">
         <v>439</v>
@@ -75387,12 +75384,12 @@
         <v>1885</v>
       </c>
       <c r="L440" t="s">
-        <v>4719</v>
+        <v>4718</v>
       </c>
     </row>
     <row r="441" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B441">
         <v>440</v>
@@ -75413,12 +75410,12 @@
         <v>1885</v>
       </c>
       <c r="L441" t="s">
-        <v>4720</v>
+        <v>4719</v>
       </c>
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B442">
         <v>441</v>
@@ -75439,12 +75436,12 @@
         <v>1885</v>
       </c>
       <c r="L442" t="s">
-        <v>4721</v>
+        <v>4720</v>
       </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B443">
         <v>442</v>
@@ -75465,12 +75462,12 @@
         <v>1885</v>
       </c>
       <c r="L443" t="s">
-        <v>4722</v>
+        <v>4721</v>
       </c>
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B444">
         <v>443</v>
@@ -75491,12 +75488,12 @@
         <v>1885</v>
       </c>
       <c r="L444" t="s">
-        <v>4723</v>
+        <v>4722</v>
       </c>
     </row>
     <row r="445" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B445">
         <v>444</v>
@@ -75517,12 +75514,12 @@
         <v>1885</v>
       </c>
       <c r="L445" t="s">
-        <v>4724</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B446">
         <v>445</v>
@@ -75546,12 +75543,12 @@
         <v>53260</v>
       </c>
       <c r="L446" t="s">
-        <v>4753</v>
+        <v>4752</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B447">
         <v>446</v>
@@ -75575,12 +75572,12 @@
         <v>53260</v>
       </c>
       <c r="L447" t="s">
-        <v>4754</v>
+        <v>4753</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B448">
         <v>447</v>
@@ -75612,7 +75609,7 @@
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B449">
         <v>448</v>
@@ -75639,12 +75636,12 @@
         <v>1537</v>
       </c>
       <c r="L449" t="s">
-        <v>4749</v>
+        <v>4748</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B450">
         <v>449</v>
@@ -75665,12 +75662,12 @@
         <v>348</v>
       </c>
       <c r="L450" t="s">
-        <v>4780</v>
+        <v>4779</v>
       </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B451">
         <v>450</v>
@@ -75691,12 +75688,12 @@
         <v>348</v>
       </c>
       <c r="L451" t="s">
-        <v>4781</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B452">
         <v>451</v>
@@ -75717,12 +75714,12 @@
         <v>348</v>
       </c>
       <c r="L452" t="s">
-        <v>4782</v>
+        <v>4781</v>
       </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B453">
         <v>452</v>
@@ -75743,12 +75740,12 @@
         <v>348</v>
       </c>
       <c r="L453" t="s">
-        <v>4783</v>
+        <v>4782</v>
       </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B454">
         <v>453</v>
@@ -75766,12 +75763,12 @@
         <v>1537</v>
       </c>
       <c r="L454" t="s">
-        <v>4779</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B455">
         <v>454</v>
@@ -75789,12 +75786,12 @@
         <v>412</v>
       </c>
       <c r="L455" t="s">
-        <v>4608</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B456">
         <v>455</v>
@@ -75812,12 +75809,12 @@
         <v>412</v>
       </c>
       <c r="L456" t="s">
-        <v>4609</v>
+        <v>4608</v>
       </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B457">
         <v>456</v>
@@ -75840,7 +75837,7 @@
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B458">
         <v>457</v>
@@ -75858,12 +75855,12 @@
         <v>412</v>
       </c>
       <c r="L458" t="s">
-        <v>4610</v>
+        <v>4609</v>
       </c>
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B459">
         <v>458</v>
@@ -75881,12 +75878,12 @@
         <v>412</v>
       </c>
       <c r="L459" t="s">
-        <v>4611</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B460">
         <v>459</v>
@@ -75910,12 +75907,12 @@
         <v>412</v>
       </c>
       <c r="L460" t="s">
-        <v>4536</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B461">
         <v>460</v>
@@ -75939,12 +75936,12 @@
         <v>412</v>
       </c>
       <c r="L461" t="s">
-        <v>4537</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="462" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B462">
         <v>461</v>
@@ -75971,12 +75968,12 @@
         <v>412</v>
       </c>
       <c r="L462" t="s">
-        <v>4693</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="463" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B463">
         <v>462</v>
@@ -76003,12 +76000,12 @@
         <v>412</v>
       </c>
       <c r="L463" t="s">
-        <v>4695</v>
+        <v>4694</v>
       </c>
     </row>
     <row r="464" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B464">
         <v>463</v>
@@ -76035,12 +76032,12 @@
         <v>412</v>
       </c>
       <c r="L464" t="s">
-        <v>4698</v>
+        <v>4697</v>
       </c>
     </row>
     <row r="465" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B465">
         <v>464</v>
@@ -76067,12 +76064,12 @@
         <v>412</v>
       </c>
       <c r="L465" t="s">
-        <v>4694</v>
+        <v>4693</v>
       </c>
     </row>
     <row r="466" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B466">
         <v>465</v>
@@ -76099,12 +76096,12 @@
         <v>412</v>
       </c>
       <c r="L466" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="467" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B467">
         <v>466</v>
@@ -76131,12 +76128,12 @@
         <v>412</v>
       </c>
       <c r="L467" t="s">
-        <v>4697</v>
+        <v>4696</v>
       </c>
     </row>
     <row r="468" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
       <c r="B468">
         <v>467</v>
@@ -76163,7 +76160,91 @@
         <v>412</v>
       </c>
       <c r="L468" t="s">
-        <v>4699</v>
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="469" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B469">
+        <v>468</v>
+      </c>
+      <c r="C469" t="s">
+        <v>420</v>
+      </c>
+      <c r="D469" t="s">
+        <v>421</v>
+      </c>
+      <c r="E469" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F469" s="1"/>
+      <c r="G469" s="1"/>
+      <c r="I469" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J469" t="s">
+        <v>412</v>
+      </c>
+      <c r="L469" t="s">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="470" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B470">
+        <v>469</v>
+      </c>
+      <c r="C470" t="s">
+        <v>423</v>
+      </c>
+      <c r="D470" t="s">
+        <v>421</v>
+      </c>
+      <c r="E470" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F470" s="1"/>
+      <c r="G470" s="1"/>
+      <c r="I470" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J470" t="s">
+        <v>412</v>
+      </c>
+      <c r="L470" t="s">
+        <v>4504</v>
+      </c>
+    </row>
+    <row r="471" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B471">
+        <v>470</v>
+      </c>
+      <c r="C471" t="s">
+        <v>424</v>
+      </c>
+      <c r="D471" t="s">
+        <v>421</v>
+      </c>
+      <c r="E471" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F471" s="1"/>
+      <c r="G471" s="1"/>
+      <c r="I471" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J471" t="s">
+        <v>412</v>
+      </c>
+      <c r="L471" t="s">
+        <v>4505</v>
       </c>
     </row>
   </sheetData>
@@ -76176,8 +76257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76222,7 +76303,7 @@
         <v>4123</v>
       </c>
       <c r="L1" t="s">
-        <v>4612</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -76463,108 +76544,6 @@
         <v>4476</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4449</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>420</v>
-      </c>
-      <c r="D10" t="s">
-        <v>421</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>412</v>
-      </c>
-      <c r="K10" t="s">
-        <v>4503</v>
-      </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-      <c r="M10" t="s">
-        <v>4506</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4449</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>423</v>
-      </c>
-      <c r="D11" t="s">
-        <v>421</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>412</v>
-      </c>
-      <c r="K11" t="s">
-        <v>4504</v>
-      </c>
-      <c r="L11">
-        <v>10</v>
-      </c>
-      <c r="M11" t="s">
-        <v>4506</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4449</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>424</v>
-      </c>
-      <c r="D12" t="s">
-        <v>421</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>412</v>
-      </c>
-      <c r="K12" t="s">
-        <v>4505</v>
-      </c>
-      <c r="L12">
-        <v>10</v>
-      </c>
-      <c r="M12" t="s">
-        <v>4506</v>
-      </c>
-    </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4449</v>
@@ -76588,13 +76567,13 @@
         <v>736</v>
       </c>
       <c r="K13" t="s">
-        <v>4507</v>
+        <v>4506</v>
       </c>
       <c r="L13">
         <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>4509</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -76620,18 +76599,18 @@
         <v>736</v>
       </c>
       <c r="K14" t="s">
-        <v>4508</v>
+        <v>4507</v>
       </c>
       <c r="L14">
         <v>11</v>
       </c>
       <c r="M14" t="s">
-        <v>4509</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -76658,18 +76637,18 @@
         <v>736</v>
       </c>
       <c r="K15" t="s">
-        <v>4618</v>
+        <v>4617</v>
       </c>
       <c r="L15">
         <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>4619</v>
+        <v>4618</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -76696,15 +76675,15 @@
         <v>3298</v>
       </c>
       <c r="K16" t="s">
-        <v>4701</v>
+        <v>4700</v>
       </c>
       <c r="M16" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -76731,15 +76710,15 @@
         <v>1537</v>
       </c>
       <c r="K17" t="s">
+        <v>4701</v>
+      </c>
+      <c r="M17" t="s">
         <v>4702</v>
-      </c>
-      <c r="M17" t="s">
-        <v>4703</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -76760,15 +76739,15 @@
         <v>515</v>
       </c>
       <c r="K18" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
       <c r="M18" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -76789,15 +76768,15 @@
         <v>515</v>
       </c>
       <c r="K19" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="M19" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -76818,15 +76797,15 @@
         <v>515</v>
       </c>
       <c r="K20" t="s">
-        <v>4706</v>
+        <v>4705</v>
       </c>
       <c r="M20" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -76850,15 +76829,15 @@
         <v>180</v>
       </c>
       <c r="K21" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
       <c r="M21" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -76882,15 +76861,15 @@
         <v>180</v>
       </c>
       <c r="K22" t="s">
-        <v>4711</v>
+        <v>4710</v>
       </c>
       <c r="M22" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -76914,15 +76893,15 @@
         <v>180</v>
       </c>
       <c r="K23" t="s">
-        <v>4712</v>
+        <v>4711</v>
       </c>
       <c r="M23" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -76946,15 +76925,15 @@
         <v>180</v>
       </c>
       <c r="K24" t="s">
-        <v>4713</v>
+        <v>4712</v>
       </c>
       <c r="M24" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -76978,15 +76957,15 @@
         <v>53260</v>
       </c>
       <c r="K25" t="s">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="M25" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -77010,15 +76989,15 @@
         <v>53260</v>
       </c>
       <c r="K26" t="s">
-        <v>4736</v>
+        <v>4735</v>
       </c>
       <c r="M26" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -77042,15 +77021,15 @@
         <v>53260</v>
       </c>
       <c r="K27" t="s">
-        <v>4737</v>
+        <v>4736</v>
       </c>
       <c r="M27" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -77074,15 +77053,15 @@
         <v>2591</v>
       </c>
       <c r="K28" t="s">
-        <v>4739</v>
+        <v>4738</v>
       </c>
       <c r="M28" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -77106,15 +77085,15 @@
         <v>2591</v>
       </c>
       <c r="K29" t="s">
-        <v>4740</v>
+        <v>4739</v>
       </c>
       <c r="M29" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -77138,15 +77117,15 @@
         <v>2591</v>
       </c>
       <c r="K30" t="s">
-        <v>4741</v>
+        <v>4740</v>
       </c>
       <c r="M30" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -77170,15 +77149,15 @@
         <v>2591</v>
       </c>
       <c r="K31" t="s">
-        <v>4742</v>
+        <v>4741</v>
       </c>
       <c r="M31" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -77196,15 +77175,15 @@
         <v>515</v>
       </c>
       <c r="K32" t="s">
-        <v>4738</v>
+        <v>4737</v>
       </c>
       <c r="M32" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -77228,15 +77207,15 @@
         <v>53260</v>
       </c>
       <c r="K33" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="M33" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -77260,15 +77239,15 @@
         <v>53260</v>
       </c>
       <c r="K34" t="s">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="M34" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -77292,15 +77271,15 @@
         <v>53260</v>
       </c>
       <c r="K35" t="s">
-        <v>4745</v>
+        <v>4744</v>
       </c>
       <c r="M35" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -77324,15 +77303,15 @@
         <v>2591</v>
       </c>
       <c r="K36" t="s">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="M36" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -77356,15 +77335,15 @@
         <v>2591</v>
       </c>
       <c r="K37" t="s">
-        <v>4747</v>
+        <v>4746</v>
       </c>
       <c r="M37" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -77388,15 +77367,15 @@
         <v>2591</v>
       </c>
       <c r="K38" t="s">
-        <v>4748</v>
+        <v>4747</v>
       </c>
       <c r="M38" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -77420,15 +77399,15 @@
         <v>180</v>
       </c>
       <c r="K39" t="s">
-        <v>4755</v>
+        <v>4754</v>
       </c>
       <c r="M39" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -77452,15 +77431,15 @@
         <v>180</v>
       </c>
       <c r="K40" t="s">
-        <v>4756</v>
+        <v>4755</v>
       </c>
       <c r="M40" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -77484,15 +77463,15 @@
         <v>180</v>
       </c>
       <c r="K41" t="s">
-        <v>4757</v>
+        <v>4756</v>
       </c>
       <c r="M41" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -77516,15 +77495,15 @@
         <v>180</v>
       </c>
       <c r="K42" t="s">
-        <v>4758</v>
+        <v>4757</v>
       </c>
       <c r="M42" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -77548,15 +77527,15 @@
         <v>180</v>
       </c>
       <c r="K43" t="s">
-        <v>4759</v>
+        <v>4758</v>
       </c>
       <c r="M43" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -77580,15 +77559,15 @@
         <v>180</v>
       </c>
       <c r="K44" t="s">
-        <v>4760</v>
+        <v>4759</v>
       </c>
       <c r="M44" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -77612,15 +77591,15 @@
         <v>180</v>
       </c>
       <c r="K45" t="s">
-        <v>4761</v>
+        <v>4760</v>
       </c>
       <c r="M45" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -77644,10 +77623,10 @@
         <v>180</v>
       </c>
       <c r="K46" t="s">
-        <v>4762</v>
+        <v>4761</v>
       </c>
       <c r="M46" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
     </row>
   </sheetData>
@@ -77752,15 +77731,15 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
+        <v>4514</v>
+      </c>
+      <c r="L3" t="s">
         <v>4515</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4516</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -77784,15 +77763,15 @@
         <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>4763</v>
+        <v>4762</v>
       </c>
       <c r="L4" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -77816,15 +77795,15 @@
         <v>180</v>
       </c>
       <c r="K5" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
       <c r="L5" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -77848,15 +77827,15 @@
         <v>180</v>
       </c>
       <c r="K6" t="s">
+        <v>4764</v>
+      </c>
+      <c r="L6" t="s">
         <v>4765</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4766</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -77877,15 +77856,15 @@
         <v>515</v>
       </c>
       <c r="K7" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="L7" t="s">
-        <v>4770</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -77906,15 +77885,15 @@
         <v>515</v>
       </c>
       <c r="K8" t="s">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="L8" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -77935,10 +77914,10 @@
         <v>515</v>
       </c>
       <c r="K9" t="s">
-        <v>4769</v>
+        <v>4768</v>
       </c>
       <c r="L9" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
     </row>
   </sheetData>
@@ -78088,7 +78067,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -78115,12 +78094,12 @@
         <v>4456</v>
       </c>
       <c r="L5" t="s">
-        <v>4622</v>
+        <v>4621</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -78147,12 +78126,12 @@
         <v>4457</v>
       </c>
       <c r="L6" t="s">
-        <v>4622</v>
+        <v>4621</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -78173,15 +78152,15 @@
         <v>1310</v>
       </c>
       <c r="K7" t="s">
-        <v>4657</v>
+        <v>4656</v>
       </c>
       <c r="L7" t="s">
-        <v>4659</v>
+        <v>4658</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -78202,15 +78181,15 @@
         <v>1310</v>
       </c>
       <c r="K8" t="s">
+        <v>4657</v>
+      </c>
+      <c r="L8" t="s">
         <v>4658</v>
-      </c>
-      <c r="L8" t="s">
-        <v>4659</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -78234,15 +78213,15 @@
         <v>180</v>
       </c>
       <c r="K9" t="s">
+        <v>4676</v>
+      </c>
+      <c r="L9" t="s">
         <v>4677</v>
-      </c>
-      <c r="L9" t="s">
-        <v>4678</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -78263,7 +78242,7 @@
         <v>1885</v>
       </c>
       <c r="K10" t="s">
-        <v>4732</v>
+        <v>4731</v>
       </c>
       <c r="L10" t="s">
         <v>4384</v>
@@ -78271,7 +78250,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -78292,7 +78271,7 @@
         <v>1885</v>
       </c>
       <c r="K11" t="s">
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="L11" t="s">
         <v>4384</v>
@@ -78300,7 +78279,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -78321,7 +78300,7 @@
         <v>1885</v>
       </c>
       <c r="K12" t="s">
-        <v>4734</v>
+        <v>4733</v>
       </c>
       <c r="L12" t="s">
         <v>4384</v>
@@ -78383,7 +78362,7 @@
         <v>4123</v>
       </c>
       <c r="L1" t="s">
-        <v>4612</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -78505,10 +78484,10 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
       <c r="M5" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -78534,10 +78513,10 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>4512</v>
+        <v>4511</v>
       </c>
       <c r="M6" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -78563,10 +78542,10 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>4513</v>
+        <v>4512</v>
       </c>
       <c r="M7" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -78592,10 +78571,10 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="M8" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -78621,15 +78600,15 @@
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>4514</v>
+        <v>4513</v>
       </c>
       <c r="M9" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -78653,15 +78632,15 @@
         <v>328</v>
       </c>
       <c r="K10" t="s">
-        <v>4539</v>
+        <v>4538</v>
       </c>
       <c r="M10" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -78685,15 +78664,15 @@
         <v>328</v>
       </c>
       <c r="K11" t="s">
-        <v>4540</v>
+        <v>4539</v>
       </c>
       <c r="M11" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -78717,15 +78696,15 @@
         <v>328</v>
       </c>
       <c r="K12" t="s">
+        <v>4540</v>
+      </c>
+      <c r="M12" t="s">
         <v>4541</v>
-      </c>
-      <c r="M12" t="s">
-        <v>4542</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -78749,15 +78728,15 @@
         <v>348</v>
       </c>
       <c r="K13" t="s">
-        <v>4552</v>
+        <v>4551</v>
       </c>
       <c r="M13" t="s">
-        <v>4561</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -78781,15 +78760,15 @@
         <v>348</v>
       </c>
       <c r="K14" t="s">
-        <v>4553</v>
+        <v>4552</v>
       </c>
       <c r="M14" t="s">
-        <v>4561</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -78813,15 +78792,15 @@
         <v>348</v>
       </c>
       <c r="K15" t="s">
-        <v>4554</v>
+        <v>4553</v>
       </c>
       <c r="M15" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -78845,15 +78824,15 @@
         <v>348</v>
       </c>
       <c r="K16" t="s">
-        <v>4555</v>
+        <v>4554</v>
       </c>
       <c r="M16" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -78877,15 +78856,15 @@
         <v>328</v>
       </c>
       <c r="K17" t="s">
-        <v>4556</v>
+        <v>4555</v>
       </c>
       <c r="M17" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -78909,15 +78888,15 @@
         <v>328</v>
       </c>
       <c r="K18" t="s">
-        <v>4557</v>
+        <v>4556</v>
       </c>
       <c r="M18" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -78941,15 +78920,15 @@
         <v>328</v>
       </c>
       <c r="K19" t="s">
-        <v>4558</v>
+        <v>4557</v>
       </c>
       <c r="M19" t="s">
-        <v>4561</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -78973,15 +78952,15 @@
         <v>348</v>
       </c>
       <c r="K20" t="s">
-        <v>4559</v>
+        <v>4558</v>
       </c>
       <c r="M20" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -79005,15 +78984,15 @@
         <v>348</v>
       </c>
       <c r="K21" t="s">
-        <v>4560</v>
+        <v>4559</v>
       </c>
       <c r="M21" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -79037,12 +79016,12 @@
         <v>3144</v>
       </c>
       <c r="M22" t="s">
-        <v>4685</v>
+        <v>4684</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -79069,10 +79048,10 @@
         <v>1537</v>
       </c>
       <c r="K23" t="s">
+        <v>4750</v>
+      </c>
+      <c r="M23" t="s">
         <v>4751</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4752</v>
       </c>
     </row>
   </sheetData>
@@ -79132,7 +79111,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -79159,15 +79138,15 @@
         <v>328</v>
       </c>
       <c r="K2" t="s">
-        <v>4546</v>
+        <v>4545</v>
       </c>
       <c r="L2" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -79194,15 +79173,15 @@
         <v>328</v>
       </c>
       <c r="K3" t="s">
+        <v>4546</v>
+      </c>
+      <c r="L3" t="s">
         <v>4547</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4548</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -79226,12 +79205,12 @@
         <v>2228</v>
       </c>
       <c r="L4" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -79255,12 +79234,12 @@
         <v>2230</v>
       </c>
       <c r="L5" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -79281,15 +79260,15 @@
         <v>186</v>
       </c>
       <c r="K6" t="s">
-        <v>4624</v>
+        <v>4623</v>
       </c>
       <c r="L6" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -79310,15 +79289,15 @@
         <v>186</v>
       </c>
       <c r="K7" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="L7" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -79339,15 +79318,15 @@
         <v>186</v>
       </c>
       <c r="K8" t="s">
-        <v>4626</v>
+        <v>4625</v>
       </c>
       <c r="L8" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -79368,15 +79347,15 @@
         <v>186</v>
       </c>
       <c r="K9" t="s">
-        <v>4627</v>
+        <v>4626</v>
       </c>
       <c r="L9" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -79397,15 +79376,15 @@
         <v>186</v>
       </c>
       <c r="K10" t="s">
-        <v>4628</v>
+        <v>4627</v>
       </c>
       <c r="L10" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -79426,15 +79405,15 @@
         <v>186</v>
       </c>
       <c r="K11" t="s">
-        <v>4629</v>
+        <v>4628</v>
       </c>
       <c r="L11" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -79455,15 +79434,15 @@
         <v>186</v>
       </c>
       <c r="K12" t="s">
-        <v>4630</v>
+        <v>4629</v>
       </c>
       <c r="L12" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -79484,15 +79463,15 @@
         <v>186</v>
       </c>
       <c r="K13" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="L13" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -79513,15 +79492,15 @@
         <v>186</v>
       </c>
       <c r="K14" t="s">
-        <v>4632</v>
+        <v>4631</v>
       </c>
       <c r="L14" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -79542,15 +79521,15 @@
         <v>186</v>
       </c>
       <c r="K15" t="s">
-        <v>4633</v>
+        <v>4632</v>
       </c>
       <c r="L15" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -79568,15 +79547,15 @@
         <v>186</v>
       </c>
       <c r="K16" t="s">
-        <v>4623</v>
+        <v>4622</v>
       </c>
       <c r="L16" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -79599,15 +79578,15 @@
       </c>
       <c r="I17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>4638</v>
+        <v>4637</v>
       </c>
       <c r="L17" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -79630,15 +79609,15 @@
       </c>
       <c r="I18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>4639</v>
+        <v>4638</v>
       </c>
       <c r="L18" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -79661,15 +79640,15 @@
       </c>
       <c r="I19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>4642</v>
+        <v>4641</v>
       </c>
       <c r="L19" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -79692,15 +79671,15 @@
       </c>
       <c r="I20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>4640</v>
+        <v>4639</v>
       </c>
       <c r="L20" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -79723,15 +79702,15 @@
       </c>
       <c r="I21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>4641</v>
+        <v>4640</v>
       </c>
       <c r="L21" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -79754,15 +79733,15 @@
       </c>
       <c r="I22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>4643</v>
+        <v>4642</v>
       </c>
       <c r="L22" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -79785,15 +79764,15 @@
       </c>
       <c r="I23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>4644</v>
+        <v>4643</v>
       </c>
       <c r="L23" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -79816,15 +79795,15 @@
       </c>
       <c r="I24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>4645</v>
+        <v>4644</v>
       </c>
       <c r="L24" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -79847,15 +79826,15 @@
       </c>
       <c r="I25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>4646</v>
+        <v>4645</v>
       </c>
       <c r="L25" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -79878,10 +79857,10 @@
       </c>
       <c r="I26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>4647</v>
+        <v>4646</v>
       </c>
       <c r="L26" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
     </row>
   </sheetData>
@@ -80081,7 +80060,7 @@
         <v>186</v>
       </c>
       <c r="L6" t="s">
-        <v>4586</v>
+        <v>4585</v>
       </c>
       <c r="M6" t="s">
         <v>4346</v>
@@ -80089,7 +80068,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -80116,15 +80095,15 @@
         <v>1537</v>
       </c>
       <c r="L7" t="s">
-        <v>4587</v>
+        <v>4586</v>
       </c>
       <c r="M7" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -80151,15 +80130,15 @@
         <v>328</v>
       </c>
       <c r="L8" t="s">
-        <v>4549</v>
+        <v>4548</v>
       </c>
       <c r="M8" t="s">
-        <v>4551</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -80186,15 +80165,15 @@
         <v>328</v>
       </c>
       <c r="L9" t="s">
+        <v>4549</v>
+      </c>
+      <c r="M9" t="s">
         <v>4550</v>
-      </c>
-      <c r="M9" t="s">
-        <v>4551</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -80218,15 +80197,15 @@
         <v>3185</v>
       </c>
       <c r="L10" t="s">
-        <v>4577</v>
+        <v>4576</v>
       </c>
       <c r="M10" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -80250,15 +80229,15 @@
         <v>3185</v>
       </c>
       <c r="L11" t="s">
-        <v>4578</v>
+        <v>4577</v>
       </c>
       <c r="M11" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -80282,15 +80261,15 @@
         <v>3185</v>
       </c>
       <c r="L12" t="s">
-        <v>4579</v>
+        <v>4578</v>
       </c>
       <c r="M12" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -80314,15 +80293,15 @@
         <v>3193</v>
       </c>
       <c r="L13" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
       <c r="M13" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -80346,15 +80325,15 @@
         <v>3193</v>
       </c>
       <c r="L14" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
       <c r="M14" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -80378,15 +80357,15 @@
         <v>3193</v>
       </c>
       <c r="L15" t="s">
-        <v>4582</v>
+        <v>4581</v>
       </c>
       <c r="M15" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -80410,15 +80389,15 @@
         <v>3193</v>
       </c>
       <c r="L16" t="s">
-        <v>4583</v>
+        <v>4582</v>
       </c>
       <c r="M16" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -80442,15 +80421,15 @@
         <v>3193</v>
       </c>
       <c r="L17" t="s">
-        <v>4584</v>
+        <v>4583</v>
       </c>
       <c r="M17" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -80474,15 +80453,15 @@
         <v>3193</v>
       </c>
       <c r="L18" t="s">
-        <v>4585</v>
+        <v>4584</v>
       </c>
       <c r="M18" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -80509,15 +80488,15 @@
         <v>1306</v>
       </c>
       <c r="L19" t="s">
-        <v>4596</v>
+        <v>4595</v>
       </c>
       <c r="M19" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -80541,12 +80520,12 @@
         <v>510</v>
       </c>
       <c r="M20" t="s">
-        <v>4620</v>
+        <v>4619</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -80570,12 +80549,12 @@
         <v>512</v>
       </c>
       <c r="M21" t="s">
-        <v>4621</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -80596,15 +80575,15 @@
         <v>1310</v>
       </c>
       <c r="L22" t="s">
-        <v>4654</v>
+        <v>4653</v>
       </c>
       <c r="M22" t="s">
-        <v>4656</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -80625,15 +80604,15 @@
         <v>1310</v>
       </c>
       <c r="L23" t="s">
+        <v>4654</v>
+      </c>
+      <c r="M23" t="s">
         <v>4655</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4656</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -80663,15 +80642,15 @@
         <v>180</v>
       </c>
       <c r="L24" t="s">
+        <v>4660</v>
+      </c>
+      <c r="M24" t="s">
         <v>4661</v>
-      </c>
-      <c r="M24" t="s">
-        <v>4662</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -80692,15 +80671,15 @@
         <v>515</v>
       </c>
       <c r="L25" t="s">
+        <v>4707</v>
+      </c>
+      <c r="M25" t="s">
         <v>4708</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4709</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -80721,15 +80700,15 @@
         <v>1885</v>
       </c>
       <c r="L26" t="s">
-        <v>4725</v>
+        <v>4724</v>
       </c>
       <c r="M26" t="s">
-        <v>4729</v>
+        <v>4728</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -80750,15 +80729,15 @@
         <v>1885</v>
       </c>
       <c r="L27" t="s">
-        <v>4726</v>
+        <v>4725</v>
       </c>
       <c r="M27" t="s">
-        <v>4730</v>
+        <v>4729</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -80779,15 +80758,15 @@
         <v>1885</v>
       </c>
       <c r="L28" t="s">
-        <v>4727</v>
+        <v>4726</v>
       </c>
       <c r="M28" t="s">
-        <v>4731</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -80808,15 +80787,15 @@
         <v>1885</v>
       </c>
       <c r="L29" t="s">
-        <v>4728</v>
+        <v>4727</v>
       </c>
       <c r="M29" t="s">
-        <v>4731</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -80840,15 +80819,15 @@
         <v>180</v>
       </c>
       <c r="L30" t="s">
-        <v>4772</v>
+        <v>4771</v>
       </c>
       <c r="M30" t="s">
-        <v>4776</v>
+        <v>4775</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -80872,15 +80851,15 @@
         <v>180</v>
       </c>
       <c r="L31" t="s">
-        <v>4773</v>
+        <v>4772</v>
       </c>
       <c r="M31" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -80904,15 +80883,15 @@
         <v>180</v>
       </c>
       <c r="L32" t="s">
-        <v>4774</v>
+        <v>4773</v>
       </c>
       <c r="M32" t="s">
-        <v>4778</v>
+        <v>4777</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -80936,10 +80915,10 @@
         <v>180</v>
       </c>
       <c r="L33" t="s">
-        <v>4775</v>
+        <v>4774</v>
       </c>
       <c r="M33" t="s">
-        <v>4778</v>
+        <v>4777</v>
       </c>
     </row>
   </sheetData>
@@ -81532,7 +81511,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -81556,12 +81535,12 @@
         <v>3193</v>
       </c>
       <c r="M22" t="s">
-        <v>4576</v>
+        <v>4575</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -81588,12 +81567,12 @@
         <v>1306</v>
       </c>
       <c r="M23" t="s">
-        <v>4595</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -81614,12 +81593,12 @@
         <v>186</v>
       </c>
       <c r="M24" t="s">
-        <v>4613</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -81645,7 +81624,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -81674,7 +81653,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -81704,12 +81683,12 @@
         <v>180</v>
       </c>
       <c r="M27" t="s">
-        <v>4660</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -81736,12 +81715,12 @@
         <v>180</v>
       </c>
       <c r="M28" t="s">
-        <v>4679</v>
+        <v>4678</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -81768,7 +81747,7 @@
         <v>3298</v>
       </c>
       <c r="M29" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sbasketb to fully working driver
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17546" uniqueCount="4784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17545" uniqueCount="4785">
   <si>
     <t>TODO</t>
   </si>
@@ -14403,6 +14403,9 @@
   </si>
   <si>
     <t>0.36.13</t>
+  </si>
+  <si>
+    <t>Super Basketball</t>
   </si>
 </sst>
 </file>
@@ -16130,8 +16133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1473"/>
   <sheetViews>
-    <sheetView topLeftCell="A1256" workbookViewId="0">
-      <selection activeCell="A1271" sqref="A1271:XFD1271"/>
+    <sheetView topLeftCell="A814" workbookViewId="0">
+      <selection activeCell="A829" sqref="A829:XFD829"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43117,41 +43120,6 @@
         <v>454</v>
       </c>
     </row>
-    <row r="829" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B829">
-        <v>838</v>
-      </c>
-      <c r="C829" t="s">
-        <v>2513</v>
-      </c>
-      <c r="D829" t="s">
-        <v>2514</v>
-      </c>
-      <c r="E829" t="s">
-        <v>3</v>
-      </c>
-      <c r="F829" t="s">
-        <v>165</v>
-      </c>
-      <c r="G829" t="s">
-        <v>166</v>
-      </c>
-      <c r="I829" t="s">
-        <v>180</v>
-      </c>
-      <c r="J829" t="s">
-        <v>2490</v>
-      </c>
-      <c r="K829" t="s">
-        <v>736</v>
-      </c>
-      <c r="L829" t="s">
-        <v>5</v>
-      </c>
-      <c r="M829" t="s">
-        <v>2515</v>
-      </c>
-    </row>
     <row r="830" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B830">
         <v>839</v>
@@ -63704,10 +63672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M471"/>
+  <dimension ref="A1:M472"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="D472" sqref="D472"/>
+      <selection activeCell="M472" sqref="M472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76245,6 +76213,38 @@
       </c>
       <c r="L471" t="s">
         <v>4505</v>
+      </c>
+    </row>
+    <row r="472" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B472">
+        <v>471</v>
+      </c>
+      <c r="C472" t="s">
+        <v>2513</v>
+      </c>
+      <c r="D472" t="s">
+        <v>2514</v>
+      </c>
+      <c r="E472" t="s">
+        <v>3</v>
+      </c>
+      <c r="F472" t="s">
+        <v>4145</v>
+      </c>
+      <c r="I472" t="s">
+        <v>180</v>
+      </c>
+      <c r="J472" t="s">
+        <v>2490</v>
+      </c>
+      <c r="K472" t="s">
+        <v>736</v>
+      </c>
+      <c r="L472" t="s">
+        <v>4784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added yiear to fully playable driver
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17527" uniqueCount="4787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17525" uniqueCount="4786">
   <si>
     <t>TODO</t>
   </si>
@@ -13557,9 +13557,6 @@
   </si>
   <si>
     <t>Yie Ar Kung-Fu (set 2)</t>
-  </si>
-  <si>
-    <t>vlm5030 has issues so it's disabled atm</t>
   </si>
   <si>
     <t>Pac-Land (set 1)</t>
@@ -15271,21 +15268,21 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="M1" s="4" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -15992,7 +15989,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16019,15 +16016,15 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>4673</v>
+        <v>4672</v>
       </c>
       <c r="N5" t="s">
-        <v>4677</v>
+        <v>4676</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16054,15 +16051,15 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
       <c r="N6" t="s">
-        <v>4677</v>
+        <v>4676</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16089,15 +16086,15 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>4675</v>
+        <v>4674</v>
       </c>
       <c r="N7" t="s">
-        <v>4677</v>
+        <v>4676</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -16124,10 +16121,10 @@
         <v>180</v>
       </c>
       <c r="M8" t="s">
+        <v>4675</v>
+      </c>
+      <c r="N8" t="s">
         <v>4676</v>
-      </c>
-      <c r="N8" t="s">
-        <v>4677</v>
       </c>
     </row>
   </sheetData>
@@ -16139,8 +16136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1473"/>
   <sheetViews>
-    <sheetView topLeftCell="A833" workbookViewId="0">
-      <selection activeCell="A848" sqref="A848:XFD849"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63374,10 +63371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M480"/>
+  <dimension ref="A1:M482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A452" workbookViewId="0">
-      <selection activeCell="M479" sqref="M479:N480"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="A483" sqref="A483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72157,7 +72154,7 @@
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B336">
         <v>335</v>
@@ -72184,12 +72181,12 @@
         <v>3180</v>
       </c>
       <c r="M336" t="s">
-        <v>4513</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B337">
         <v>336</v>
@@ -72213,15 +72210,15 @@
         <v>328</v>
       </c>
       <c r="L337" t="s">
+        <v>4511</v>
+      </c>
+      <c r="M337" t="s">
         <v>4512</v>
-      </c>
-      <c r="M337" t="s">
-        <v>4513</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B338">
         <v>337</v>
@@ -72242,15 +72239,15 @@
         <v>1309</v>
       </c>
       <c r="L338" t="s">
-        <v>4514</v>
+        <v>4513</v>
       </c>
       <c r="M338" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B339">
         <v>338</v>
@@ -72271,15 +72268,15 @@
         <v>1309</v>
       </c>
       <c r="L339" t="s">
-        <v>4515</v>
+        <v>4514</v>
       </c>
       <c r="M339" t="s">
-        <v>4517</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B340">
         <v>339</v>
@@ -72300,15 +72297,15 @@
         <v>1309</v>
       </c>
       <c r="L340" t="s">
+        <v>4515</v>
+      </c>
+      <c r="M340" t="s">
         <v>4516</v>
-      </c>
-      <c r="M340" t="s">
-        <v>4517</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B341">
         <v>340</v>
@@ -72334,12 +72331,12 @@
         <v>329</v>
       </c>
       <c r="L341" t="s">
-        <v>4518</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B342">
         <v>341</v>
@@ -72365,12 +72362,12 @@
         <v>329</v>
       </c>
       <c r="L342" t="s">
-        <v>4519</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B343">
         <v>342</v>
@@ -72396,12 +72393,12 @@
         <v>329</v>
       </c>
       <c r="L343" t="s">
-        <v>4520</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B344">
         <v>343</v>
@@ -72427,12 +72424,12 @@
         <v>329</v>
       </c>
       <c r="L344" t="s">
-        <v>4521</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B345">
         <v>344</v>
@@ -72458,12 +72455,12 @@
         <v>329</v>
       </c>
       <c r="L345" t="s">
-        <v>4522</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B346">
         <v>345</v>
@@ -72489,12 +72486,12 @@
         <v>329</v>
       </c>
       <c r="L346" t="s">
-        <v>4523</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B347">
         <v>346</v>
@@ -72520,12 +72517,12 @@
         <v>329</v>
       </c>
       <c r="L347" t="s">
-        <v>4524</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B348">
         <v>347</v>
@@ -72549,12 +72546,12 @@
         <v>180</v>
       </c>
       <c r="L348" t="s">
-        <v>4525</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B349">
         <v>348</v>
@@ -72578,12 +72575,12 @@
         <v>180</v>
       </c>
       <c r="L349" t="s">
-        <v>4527</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B350">
         <v>349</v>
@@ -72607,12 +72604,12 @@
         <v>180</v>
       </c>
       <c r="L350" t="s">
-        <v>4526</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B351">
         <v>350</v>
@@ -72636,12 +72633,12 @@
         <v>180</v>
       </c>
       <c r="L351" t="s">
-        <v>4528</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B352">
         <v>351</v>
@@ -72668,12 +72665,12 @@
         <v>328</v>
       </c>
       <c r="L352" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B353">
         <v>352</v>
@@ -72700,12 +72697,12 @@
         <v>328</v>
       </c>
       <c r="L353" t="s">
-        <v>4537</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B354">
         <v>353</v>
@@ -72735,12 +72732,12 @@
         <v>1305</v>
       </c>
       <c r="L354" t="s">
-        <v>4536</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B355">
         <v>354</v>
@@ -72764,12 +72761,12 @@
         <v>87</v>
       </c>
       <c r="L355" t="s">
-        <v>4555</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B356">
         <v>355</v>
@@ -72793,12 +72790,12 @@
         <v>87</v>
       </c>
       <c r="L356" t="s">
-        <v>4556</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B357">
         <v>356</v>
@@ -72822,12 +72819,12 @@
         <v>87</v>
       </c>
       <c r="L357" t="s">
-        <v>4557</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B358">
         <v>357</v>
@@ -72851,12 +72848,12 @@
         <v>87</v>
       </c>
       <c r="L358" t="s">
-        <v>4558</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B359">
         <v>358</v>
@@ -72880,12 +72877,12 @@
         <v>87</v>
       </c>
       <c r="L359" t="s">
-        <v>4559</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B360">
         <v>359</v>
@@ -72909,12 +72906,12 @@
         <v>87</v>
       </c>
       <c r="L360" t="s">
-        <v>4560</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B361">
         <v>360</v>
@@ -72938,12 +72935,12 @@
         <v>87</v>
       </c>
       <c r="L361" t="s">
-        <v>4561</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B362">
         <v>361</v>
@@ -72967,12 +72964,12 @@
         <v>87</v>
       </c>
       <c r="L362" t="s">
-        <v>4562</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B363">
         <v>362</v>
@@ -72996,12 +72993,12 @@
         <v>87</v>
       </c>
       <c r="L363" t="s">
-        <v>4563</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B364">
         <v>363</v>
@@ -73025,12 +73022,12 @@
         <v>87</v>
       </c>
       <c r="L364" t="s">
-        <v>4564</v>
+        <v>4563</v>
       </c>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B365">
         <v>364</v>
@@ -73054,12 +73051,12 @@
         <v>87</v>
       </c>
       <c r="L365" t="s">
-        <v>4565</v>
+        <v>4564</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B366">
         <v>365</v>
@@ -73083,12 +73080,12 @@
         <v>87</v>
       </c>
       <c r="L366" t="s">
-        <v>4566</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B367">
         <v>366</v>
@@ -73111,12 +73108,12 @@
         <v>186</v>
       </c>
       <c r="L367" t="s">
-        <v>4567</v>
+        <v>4566</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B368">
         <v>367</v>
@@ -73139,12 +73136,12 @@
         <v>186</v>
       </c>
       <c r="L368" t="s">
-        <v>4568</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B369">
         <v>368</v>
@@ -73172,7 +73169,7 @@
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B370">
         <v>369</v>
@@ -73197,12 +73194,12 @@
         <v>3187</v>
       </c>
       <c r="L370" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B371">
         <v>370</v>
@@ -73227,12 +73224,12 @@
         <v>3187</v>
       </c>
       <c r="L371" t="s">
-        <v>4582</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="372" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B372">
         <v>371</v>
@@ -73257,12 +73254,12 @@
         <v>3187</v>
       </c>
       <c r="L372" t="s">
-        <v>4583</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="373" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B373">
         <v>372</v>
@@ -73287,12 +73284,12 @@
         <v>3187</v>
       </c>
       <c r="L373" t="s">
-        <v>4584</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B374">
         <v>373</v>
@@ -73317,12 +73314,12 @@
         <v>3187</v>
       </c>
       <c r="L374" t="s">
-        <v>4585</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B375">
         <v>374</v>
@@ -73350,12 +73347,12 @@
         <v>3201</v>
       </c>
       <c r="L375" t="s">
-        <v>4586</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="376" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B376">
         <v>375</v>
@@ -73383,12 +73380,12 @@
         <v>3201</v>
       </c>
       <c r="L376" t="s">
-        <v>4587</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B377">
         <v>376</v>
@@ -73415,12 +73412,12 @@
         <v>1305</v>
       </c>
       <c r="L377" t="s">
-        <v>4591</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="378" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B378">
         <v>377</v>
@@ -73441,12 +73438,12 @@
         <v>323</v>
       </c>
       <c r="L378" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B379">
         <v>378</v>
@@ -73472,7 +73469,7 @@
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B380">
         <v>379</v>
@@ -73490,12 +73487,12 @@
         <v>2868</v>
       </c>
       <c r="L380" t="s">
-        <v>4593</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="381" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B381">
         <v>380</v>
@@ -73513,12 +73510,12 @@
         <v>2868</v>
       </c>
       <c r="L381" t="s">
-        <v>4594</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B382">
         <v>381</v>
@@ -73536,12 +73533,12 @@
         <v>2868</v>
       </c>
       <c r="L382" t="s">
-        <v>4595</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B383">
         <v>382</v>
@@ -73567,7 +73564,7 @@
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B384">
         <v>383</v>
@@ -73593,7 +73590,7 @@
     </row>
     <row r="385" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B385">
         <v>384</v>
@@ -73611,12 +73608,12 @@
         <v>74</v>
       </c>
       <c r="L385" t="s">
-        <v>4596</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B386">
         <v>385</v>
@@ -73634,12 +73631,12 @@
         <v>74</v>
       </c>
       <c r="L386" t="s">
-        <v>4597</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B387">
         <v>386</v>
@@ -73657,12 +73654,12 @@
         <v>74</v>
       </c>
       <c r="L387" t="s">
-        <v>4598</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B388">
         <v>387</v>
@@ -73682,7 +73679,7 @@
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B389">
         <v>388</v>
@@ -73708,7 +73705,7 @@
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B390">
         <v>389</v>
@@ -73734,7 +73731,7 @@
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B391">
         <v>390</v>
@@ -73752,12 +73749,12 @@
         <v>74</v>
       </c>
       <c r="L391" t="s">
-        <v>4607</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B392">
         <v>391</v>
@@ -73780,7 +73777,7 @@
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B393">
         <v>392</v>
@@ -73803,7 +73800,7 @@
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B394">
         <v>393</v>
@@ -73826,7 +73823,7 @@
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B395">
         <v>394</v>
@@ -73844,12 +73841,12 @@
         <v>74</v>
       </c>
       <c r="L395" t="s">
-        <v>4608</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B396">
         <v>395</v>
@@ -73867,12 +73864,12 @@
         <v>74</v>
       </c>
       <c r="L396" t="s">
-        <v>4609</v>
+        <v>4608</v>
       </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B397">
         <v>396</v>
@@ -73890,12 +73887,12 @@
         <v>74</v>
       </c>
       <c r="L397" t="s">
-        <v>4610</v>
+        <v>4609</v>
       </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B398">
         <v>397</v>
@@ -73918,7 +73915,7 @@
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B399">
         <v>398</v>
@@ -73936,12 +73933,12 @@
         <v>2872</v>
       </c>
       <c r="L399" t="s">
-        <v>4599</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B400">
         <v>399</v>
@@ -73959,12 +73956,12 @@
         <v>2872</v>
       </c>
       <c r="L400" t="s">
-        <v>4600</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B401">
         <v>400</v>
@@ -73982,12 +73979,12 @@
         <v>2868</v>
       </c>
       <c r="L401" t="s">
-        <v>4627</v>
+        <v>4626</v>
       </c>
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B402">
         <v>401</v>
@@ -74005,12 +74002,12 @@
         <v>2868</v>
       </c>
       <c r="L402" t="s">
-        <v>4628</v>
+        <v>4627</v>
       </c>
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B403">
         <v>402</v>
@@ -74028,12 +74025,12 @@
         <v>74</v>
       </c>
       <c r="L403" t="s">
-        <v>4629</v>
+        <v>4628</v>
       </c>
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B404">
         <v>403</v>
@@ -74051,12 +74048,12 @@
         <v>74</v>
       </c>
       <c r="L404" t="s">
-        <v>4630</v>
+        <v>4629</v>
       </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B405">
         <v>404</v>
@@ -74074,12 +74071,12 @@
         <v>186</v>
       </c>
       <c r="L405" t="s">
-        <v>4641</v>
+        <v>4640</v>
       </c>
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B406">
         <v>405</v>
@@ -74102,12 +74099,12 @@
         <v>186</v>
       </c>
       <c r="L406" t="s">
-        <v>4642</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B407">
         <v>406</v>
@@ -74130,12 +74127,12 @@
         <v>186</v>
       </c>
       <c r="L407" t="s">
-        <v>4643</v>
+        <v>4642</v>
       </c>
     </row>
     <row r="408" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B408">
         <v>407</v>
@@ -74156,12 +74153,12 @@
         <v>74</v>
       </c>
       <c r="L408" t="s">
-        <v>4644</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="409" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B409">
         <v>408</v>
@@ -74187,7 +74184,7 @@
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B410">
         <v>409</v>
@@ -74208,12 +74205,12 @@
         <v>74</v>
       </c>
       <c r="L410" t="s">
-        <v>4645</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B411">
         <v>410</v>
@@ -74239,7 +74236,7 @@
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B412">
         <v>411</v>
@@ -74260,12 +74257,12 @@
         <v>74</v>
       </c>
       <c r="L412" t="s">
-        <v>4646</v>
+        <v>4645</v>
       </c>
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B413">
         <v>412</v>
@@ -74295,12 +74292,12 @@
         <v>180</v>
       </c>
       <c r="L413" t="s">
-        <v>4656</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B414">
         <v>413</v>
@@ -74330,12 +74327,12 @@
         <v>180</v>
       </c>
       <c r="L414" t="s">
-        <v>4657</v>
+        <v>4656</v>
       </c>
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B415">
         <v>414</v>
@@ -74359,12 +74356,12 @@
         <v>180</v>
       </c>
       <c r="L415" t="s">
-        <v>4658</v>
+        <v>4657</v>
       </c>
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B416">
         <v>415</v>
@@ -74388,12 +74385,12 @@
         <v>180</v>
       </c>
       <c r="L416" t="s">
-        <v>4659</v>
+        <v>4658</v>
       </c>
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B417">
         <v>416</v>
@@ -74417,12 +74414,12 @@
         <v>180</v>
       </c>
       <c r="L417" t="s">
-        <v>4660</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="418" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B418">
         <v>417</v>
@@ -74446,12 +74443,12 @@
         <v>180</v>
       </c>
       <c r="L418" t="s">
-        <v>4661</v>
+        <v>4660</v>
       </c>
     </row>
     <row r="419" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B419">
         <v>418</v>
@@ -74475,12 +74472,12 @@
         <v>180</v>
       </c>
       <c r="L419" t="s">
-        <v>4662</v>
+        <v>4661</v>
       </c>
     </row>
     <row r="420" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B420">
         <v>419</v>
@@ -74504,12 +74501,12 @@
         <v>180</v>
       </c>
       <c r="L420" t="s">
-        <v>4663</v>
+        <v>4662</v>
       </c>
     </row>
     <row r="421" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B421">
         <v>420</v>
@@ -74533,12 +74530,12 @@
         <v>180</v>
       </c>
       <c r="L421" t="s">
-        <v>4664</v>
+        <v>4663</v>
       </c>
     </row>
     <row r="422" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B422">
         <v>421</v>
@@ -74562,12 +74559,12 @@
         <v>180</v>
       </c>
       <c r="L422" t="s">
-        <v>4666</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="423" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B423">
         <v>422</v>
@@ -74591,12 +74588,12 @@
         <v>180</v>
       </c>
       <c r="L423" t="s">
-        <v>4665</v>
+        <v>4664</v>
       </c>
     </row>
     <row r="424" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B424">
         <v>423</v>
@@ -74620,12 +74617,12 @@
         <v>180</v>
       </c>
       <c r="L424" t="s">
-        <v>4667</v>
+        <v>4666</v>
       </c>
     </row>
     <row r="425" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B425">
         <v>424</v>
@@ -74649,12 +74646,12 @@
         <v>180</v>
       </c>
       <c r="L425" t="s">
-        <v>4668</v>
+        <v>4667</v>
       </c>
     </row>
     <row r="426" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B426">
         <v>425</v>
@@ -74678,12 +74675,12 @@
         <v>180</v>
       </c>
       <c r="L426" t="s">
-        <v>4669</v>
+        <v>4668</v>
       </c>
     </row>
     <row r="427" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B427">
         <v>426</v>
@@ -74704,12 +74701,12 @@
         <v>186</v>
       </c>
       <c r="L427" t="s">
-        <v>4679</v>
+        <v>4678</v>
       </c>
     </row>
     <row r="428" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B428">
         <v>427</v>
@@ -74730,12 +74727,12 @@
         <v>186</v>
       </c>
       <c r="L428" t="s">
-        <v>4680</v>
+        <v>4679</v>
       </c>
     </row>
     <row r="429" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B429">
         <v>428</v>
@@ -74759,12 +74756,12 @@
         <v>180</v>
       </c>
       <c r="L429" t="s">
-        <v>4681</v>
+        <v>4680</v>
       </c>
     </row>
     <row r="430" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B430">
         <v>429</v>
@@ -74788,12 +74785,12 @@
         <v>180</v>
       </c>
       <c r="L430" t="s">
-        <v>4682</v>
+        <v>4681</v>
       </c>
     </row>
     <row r="431" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B431">
         <v>430</v>
@@ -74817,12 +74814,12 @@
         <v>1305</v>
       </c>
       <c r="L431" t="s">
-        <v>4683</v>
+        <v>4682</v>
       </c>
     </row>
     <row r="432" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B432">
         <v>431</v>
@@ -74846,12 +74843,12 @@
         <v>1305</v>
       </c>
       <c r="L432" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="433" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B433">
         <v>432</v>
@@ -74877,7 +74874,7 @@
     </row>
     <row r="434" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B434">
         <v>433</v>
@@ -74898,12 +74895,12 @@
         <v>186</v>
       </c>
       <c r="L434" t="s">
-        <v>4685</v>
+        <v>4684</v>
       </c>
     </row>
     <row r="435" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B435">
         <v>434</v>
@@ -74924,12 +74921,12 @@
         <v>1884</v>
       </c>
       <c r="L435" t="s">
-        <v>4707</v>
+        <v>4706</v>
       </c>
     </row>
     <row r="436" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B436">
         <v>435</v>
@@ -74950,12 +74947,12 @@
         <v>1884</v>
       </c>
       <c r="L436" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
     </row>
     <row r="437" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B437">
         <v>436</v>
@@ -74976,12 +74973,12 @@
         <v>1884</v>
       </c>
       <c r="L437" t="s">
-        <v>4709</v>
+        <v>4708</v>
       </c>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B438">
         <v>437</v>
@@ -75002,12 +74999,12 @@
         <v>1884</v>
       </c>
       <c r="L438" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
     </row>
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B439">
         <v>438</v>
@@ -75028,12 +75025,12 @@
         <v>1884</v>
       </c>
       <c r="L439" t="s">
-        <v>4711</v>
+        <v>4710</v>
       </c>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B440">
         <v>439</v>
@@ -75054,12 +75051,12 @@
         <v>1884</v>
       </c>
       <c r="L440" t="s">
-        <v>4712</v>
+        <v>4711</v>
       </c>
     </row>
     <row r="441" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B441">
         <v>440</v>
@@ -75080,12 +75077,12 @@
         <v>1884</v>
       </c>
       <c r="L441" t="s">
-        <v>4713</v>
+        <v>4712</v>
       </c>
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B442">
         <v>441</v>
@@ -75106,12 +75103,12 @@
         <v>1884</v>
       </c>
       <c r="L442" t="s">
-        <v>4714</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B443">
         <v>442</v>
@@ -75132,12 +75129,12 @@
         <v>1884</v>
       </c>
       <c r="L443" t="s">
-        <v>4715</v>
+        <v>4714</v>
       </c>
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B444">
         <v>443</v>
@@ -75158,12 +75155,12 @@
         <v>1884</v>
       </c>
       <c r="L444" t="s">
-        <v>4716</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="445" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B445">
         <v>444</v>
@@ -75184,12 +75181,12 @@
         <v>1884</v>
       </c>
       <c r="L445" t="s">
-        <v>4717</v>
+        <v>4716</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B446">
         <v>445</v>
@@ -75213,12 +75210,12 @@
         <v>53260</v>
       </c>
       <c r="L446" t="s">
-        <v>4746</v>
+        <v>4745</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B447">
         <v>446</v>
@@ -75242,12 +75239,12 @@
         <v>53260</v>
       </c>
       <c r="L447" t="s">
-        <v>4747</v>
+        <v>4746</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B448">
         <v>447</v>
@@ -75279,7 +75276,7 @@
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B449">
         <v>448</v>
@@ -75306,12 +75303,12 @@
         <v>1536</v>
       </c>
       <c r="L449" t="s">
-        <v>4742</v>
+        <v>4741</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B450">
         <v>449</v>
@@ -75332,12 +75329,12 @@
         <v>348</v>
       </c>
       <c r="L450" t="s">
-        <v>4773</v>
+        <v>4772</v>
       </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B451">
         <v>450</v>
@@ -75358,12 +75355,12 @@
         <v>348</v>
       </c>
       <c r="L451" t="s">
-        <v>4774</v>
+        <v>4773</v>
       </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B452">
         <v>451</v>
@@ -75384,12 +75381,12 @@
         <v>348</v>
       </c>
       <c r="L452" t="s">
-        <v>4775</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B453">
         <v>452</v>
@@ -75410,12 +75407,12 @@
         <v>348</v>
       </c>
       <c r="L453" t="s">
-        <v>4776</v>
+        <v>4775</v>
       </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B454">
         <v>453</v>
@@ -75433,12 +75430,12 @@
         <v>1536</v>
       </c>
       <c r="L454" t="s">
-        <v>4772</v>
+        <v>4771</v>
       </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B455">
         <v>454</v>
@@ -75456,12 +75453,12 @@
         <v>412</v>
       </c>
       <c r="L455" t="s">
-        <v>4601</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B456">
         <v>455</v>
@@ -75479,12 +75476,12 @@
         <v>412</v>
       </c>
       <c r="L456" t="s">
-        <v>4602</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B457">
         <v>456</v>
@@ -75507,7 +75504,7 @@
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B458">
         <v>457</v>
@@ -75525,12 +75522,12 @@
         <v>412</v>
       </c>
       <c r="L458" t="s">
-        <v>4603</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B459">
         <v>458</v>
@@ -75548,12 +75545,12 @@
         <v>412</v>
       </c>
       <c r="L459" t="s">
-        <v>4604</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B460">
         <v>459</v>
@@ -75577,12 +75574,12 @@
         <v>412</v>
       </c>
       <c r="L460" t="s">
-        <v>4529</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B461">
         <v>460</v>
@@ -75606,12 +75603,12 @@
         <v>412</v>
       </c>
       <c r="L461" t="s">
-        <v>4530</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="462" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B462">
         <v>461</v>
@@ -75638,12 +75635,12 @@
         <v>412</v>
       </c>
       <c r="L462" t="s">
-        <v>4686</v>
+        <v>4685</v>
       </c>
     </row>
     <row r="463" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B463">
         <v>462</v>
@@ -75670,12 +75667,12 @@
         <v>412</v>
       </c>
       <c r="L463" t="s">
-        <v>4688</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="464" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B464">
         <v>463</v>
@@ -75702,12 +75699,12 @@
         <v>412</v>
       </c>
       <c r="L464" t="s">
-        <v>4691</v>
+        <v>4690</v>
       </c>
     </row>
     <row r="465" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B465">
         <v>464</v>
@@ -75734,12 +75731,12 @@
         <v>412</v>
       </c>
       <c r="L465" t="s">
-        <v>4687</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="466" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B466">
         <v>465</v>
@@ -75766,12 +75763,12 @@
         <v>412</v>
       </c>
       <c r="L466" t="s">
-        <v>4689</v>
+        <v>4688</v>
       </c>
     </row>
     <row r="467" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B467">
         <v>466</v>
@@ -75798,12 +75795,12 @@
         <v>412</v>
       </c>
       <c r="L467" t="s">
-        <v>4690</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="468" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B468">
         <v>467</v>
@@ -75830,12 +75827,12 @@
         <v>412</v>
       </c>
       <c r="L468" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
     </row>
     <row r="469" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B469">
         <v>468</v>
@@ -75863,7 +75860,7 @@
     </row>
     <row r="470" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B470">
         <v>469</v>
@@ -75891,7 +75888,7 @@
     </row>
     <row r="471" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B471">
         <v>470</v>
@@ -75919,7 +75916,7 @@
     </row>
     <row r="472" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B472">
         <v>471</v>
@@ -75946,12 +75943,12 @@
         <v>735</v>
       </c>
       <c r="L472" t="s">
-        <v>4778</v>
+        <v>4777</v>
       </c>
     </row>
     <row r="473" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B473">
         <v>472</v>
@@ -75978,12 +75975,12 @@
         <v>735</v>
       </c>
       <c r="L473" t="s">
-        <v>4779</v>
+        <v>4778</v>
       </c>
     </row>
     <row r="474" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B474">
         <v>473</v>
@@ -76010,12 +76007,12 @@
         <v>735</v>
       </c>
       <c r="L474" t="s">
-        <v>4780</v>
+        <v>4779</v>
       </c>
     </row>
     <row r="475" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B475">
         <v>474</v>
@@ -76042,12 +76039,12 @@
         <v>735</v>
       </c>
       <c r="L475" t="s">
-        <v>4781</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="476" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B476">
         <v>475</v>
@@ -76074,12 +76071,12 @@
         <v>735</v>
       </c>
       <c r="L476" t="s">
-        <v>4782</v>
+        <v>4781</v>
       </c>
     </row>
     <row r="477" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B477">
         <v>476</v>
@@ -76106,12 +76103,12 @@
         <v>735</v>
       </c>
       <c r="L477" t="s">
-        <v>4783</v>
+        <v>4782</v>
       </c>
     </row>
     <row r="478" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B478">
         <v>477</v>
@@ -76138,12 +76135,12 @@
         <v>735</v>
       </c>
       <c r="L478" t="s">
-        <v>4784</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="479" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B479">
         <v>478</v>
@@ -76167,12 +76164,12 @@
         <v>735</v>
       </c>
       <c r="L479" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="480" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="B480">
         <v>479</v>
@@ -76196,7 +76193,59 @@
         <v>735</v>
       </c>
       <c r="L480" t="s">
-        <v>4786</v>
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="481" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>4776</v>
+      </c>
+      <c r="B481">
+        <v>480</v>
+      </c>
+      <c r="C481" t="s">
+        <v>2522</v>
+      </c>
+      <c r="D481" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E481" t="s">
+        <v>3</v>
+      </c>
+      <c r="I481" t="s">
+        <v>2489</v>
+      </c>
+      <c r="J481" t="s">
+        <v>735</v>
+      </c>
+      <c r="L481" t="s">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="482" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>4776</v>
+      </c>
+      <c r="B482">
+        <v>481</v>
+      </c>
+      <c r="C482" t="s">
+        <v>2524</v>
+      </c>
+      <c r="D482" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E482" t="s">
+        <v>3</v>
+      </c>
+      <c r="I482" t="s">
+        <v>2489</v>
+      </c>
+      <c r="J482" t="s">
+        <v>735</v>
+      </c>
+      <c r="L482" t="s">
+        <v>4501</v>
       </c>
     </row>
   </sheetData>
@@ -76209,8 +76258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76255,7 +76304,7 @@
         <v>4117</v>
       </c>
       <c r="L1" t="s">
-        <v>4605</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -76496,73 +76545,9 @@
         <v>4470</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4443</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2522</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2523</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" t="s">
-        <v>2489</v>
-      </c>
-      <c r="I13" t="s">
-        <v>735</v>
-      </c>
-      <c r="K13" t="s">
-        <v>4500</v>
-      </c>
-      <c r="L13">
-        <v>11</v>
-      </c>
-      <c r="M13" t="s">
-        <v>4502</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4443</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2524</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2523</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" t="s">
-        <v>2489</v>
-      </c>
-      <c r="I14" t="s">
-        <v>735</v>
-      </c>
-      <c r="K14" t="s">
-        <v>4501</v>
-      </c>
-      <c r="L14">
-        <v>11</v>
-      </c>
-      <c r="M14" t="s">
-        <v>4502</v>
-      </c>
-    </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -76589,18 +76574,18 @@
         <v>735</v>
       </c>
       <c r="K15" t="s">
-        <v>4611</v>
+        <v>4610</v>
       </c>
       <c r="L15">
         <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>4612</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -76627,15 +76612,15 @@
         <v>3292</v>
       </c>
       <c r="K16" t="s">
-        <v>4694</v>
+        <v>4693</v>
       </c>
       <c r="M16" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -76662,15 +76647,15 @@
         <v>1536</v>
       </c>
       <c r="K17" t="s">
+        <v>4694</v>
+      </c>
+      <c r="M17" t="s">
         <v>4695</v>
-      </c>
-      <c r="M17" t="s">
-        <v>4696</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -76691,15 +76676,15 @@
         <v>514</v>
       </c>
       <c r="K18" t="s">
-        <v>4697</v>
+        <v>4696</v>
       </c>
       <c r="M18" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -76720,15 +76705,15 @@
         <v>514</v>
       </c>
       <c r="K19" t="s">
-        <v>4698</v>
+        <v>4697</v>
       </c>
       <c r="M19" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -76749,15 +76734,15 @@
         <v>514</v>
       </c>
       <c r="K20" t="s">
-        <v>4699</v>
+        <v>4698</v>
       </c>
       <c r="M20" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -76781,15 +76766,15 @@
         <v>180</v>
       </c>
       <c r="K21" t="s">
-        <v>4703</v>
+        <v>4702</v>
       </c>
       <c r="M21" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -76813,15 +76798,15 @@
         <v>180</v>
       </c>
       <c r="K22" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
       <c r="M22" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -76845,15 +76830,15 @@
         <v>180</v>
       </c>
       <c r="K23" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="M23" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -76877,15 +76862,15 @@
         <v>180</v>
       </c>
       <c r="K24" t="s">
-        <v>4706</v>
+        <v>4705</v>
       </c>
       <c r="M24" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -76909,15 +76894,15 @@
         <v>53260</v>
       </c>
       <c r="K25" t="s">
-        <v>4728</v>
+        <v>4727</v>
       </c>
       <c r="M25" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -76941,15 +76926,15 @@
         <v>53260</v>
       </c>
       <c r="K26" t="s">
-        <v>4729</v>
+        <v>4728</v>
       </c>
       <c r="M26" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -76973,15 +76958,15 @@
         <v>53260</v>
       </c>
       <c r="K27" t="s">
-        <v>4730</v>
+        <v>4729</v>
       </c>
       <c r="M27" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -77005,15 +76990,15 @@
         <v>2585</v>
       </c>
       <c r="K28" t="s">
-        <v>4732</v>
+        <v>4731</v>
       </c>
       <c r="M28" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -77037,15 +77022,15 @@
         <v>2585</v>
       </c>
       <c r="K29" t="s">
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="M29" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -77069,15 +77054,15 @@
         <v>2585</v>
       </c>
       <c r="K30" t="s">
-        <v>4734</v>
+        <v>4733</v>
       </c>
       <c r="M30" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -77101,15 +77086,15 @@
         <v>2585</v>
       </c>
       <c r="K31" t="s">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="M31" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -77127,15 +77112,15 @@
         <v>514</v>
       </c>
       <c r="K32" t="s">
-        <v>4731</v>
+        <v>4730</v>
       </c>
       <c r="M32" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -77159,15 +77144,15 @@
         <v>53260</v>
       </c>
       <c r="K33" t="s">
-        <v>4736</v>
+        <v>4735</v>
       </c>
       <c r="M33" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -77191,15 +77176,15 @@
         <v>53260</v>
       </c>
       <c r="K34" t="s">
-        <v>4737</v>
+        <v>4736</v>
       </c>
       <c r="M34" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -77223,15 +77208,15 @@
         <v>53260</v>
       </c>
       <c r="K35" t="s">
-        <v>4738</v>
+        <v>4737</v>
       </c>
       <c r="M35" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -77255,15 +77240,15 @@
         <v>2585</v>
       </c>
       <c r="K36" t="s">
-        <v>4739</v>
+        <v>4738</v>
       </c>
       <c r="M36" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -77287,15 +77272,15 @@
         <v>2585</v>
       </c>
       <c r="K37" t="s">
-        <v>4740</v>
+        <v>4739</v>
       </c>
       <c r="M37" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -77319,15 +77304,15 @@
         <v>2585</v>
       </c>
       <c r="K38" t="s">
-        <v>4741</v>
+        <v>4740</v>
       </c>
       <c r="M38" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -77351,15 +77336,15 @@
         <v>180</v>
       </c>
       <c r="K39" t="s">
-        <v>4748</v>
+        <v>4747</v>
       </c>
       <c r="M39" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -77383,15 +77368,15 @@
         <v>180</v>
       </c>
       <c r="K40" t="s">
-        <v>4749</v>
+        <v>4748</v>
       </c>
       <c r="M40" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -77415,15 +77400,15 @@
         <v>180</v>
       </c>
       <c r="K41" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="M41" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -77447,15 +77432,15 @@
         <v>180</v>
       </c>
       <c r="K42" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="M42" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -77479,15 +77464,15 @@
         <v>180</v>
       </c>
       <c r="K43" t="s">
-        <v>4752</v>
+        <v>4751</v>
       </c>
       <c r="M43" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -77511,15 +77496,15 @@
         <v>180</v>
       </c>
       <c r="K44" t="s">
-        <v>4753</v>
+        <v>4752</v>
       </c>
       <c r="M44" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -77543,15 +77528,15 @@
         <v>180</v>
       </c>
       <c r="K45" t="s">
-        <v>4754</v>
+        <v>4753</v>
       </c>
       <c r="M45" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -77575,10 +77560,10 @@
         <v>180</v>
       </c>
       <c r="K46" t="s">
-        <v>4755</v>
+        <v>4754</v>
       </c>
       <c r="M46" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
     </row>
   </sheetData>
@@ -77683,15 +77668,15 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
+        <v>4507</v>
+      </c>
+      <c r="L3" t="s">
         <v>4508</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4509</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -77715,15 +77700,15 @@
         <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>4756</v>
+        <v>4755</v>
       </c>
       <c r="L4" t="s">
-        <v>4759</v>
+        <v>4758</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -77747,15 +77732,15 @@
         <v>180</v>
       </c>
       <c r="K5" t="s">
-        <v>4757</v>
+        <v>4756</v>
       </c>
       <c r="L5" t="s">
-        <v>4759</v>
+        <v>4758</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -77779,15 +77764,15 @@
         <v>180</v>
       </c>
       <c r="K6" t="s">
+        <v>4757</v>
+      </c>
+      <c r="L6" t="s">
         <v>4758</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4759</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -77808,15 +77793,15 @@
         <v>514</v>
       </c>
       <c r="K7" t="s">
-        <v>4760</v>
+        <v>4759</v>
       </c>
       <c r="L7" t="s">
-        <v>4763</v>
+        <v>4762</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -77837,15 +77822,15 @@
         <v>514</v>
       </c>
       <c r="K8" t="s">
-        <v>4761</v>
+        <v>4760</v>
       </c>
       <c r="L8" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -77866,10 +77851,10 @@
         <v>514</v>
       </c>
       <c r="K9" t="s">
-        <v>4762</v>
+        <v>4761</v>
       </c>
       <c r="L9" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
     </row>
   </sheetData>
@@ -78019,7 +78004,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -78046,12 +78031,12 @@
         <v>4450</v>
       </c>
       <c r="L5" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -78078,12 +78063,12 @@
         <v>4451</v>
       </c>
       <c r="L6" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -78104,15 +78089,15 @@
         <v>1309</v>
       </c>
       <c r="K7" t="s">
-        <v>4650</v>
+        <v>4649</v>
       </c>
       <c r="L7" t="s">
-        <v>4652</v>
+        <v>4651</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -78133,15 +78118,15 @@
         <v>1309</v>
       </c>
       <c r="K8" t="s">
+        <v>4650</v>
+      </c>
+      <c r="L8" t="s">
         <v>4651</v>
-      </c>
-      <c r="L8" t="s">
-        <v>4652</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -78165,15 +78150,15 @@
         <v>180</v>
       </c>
       <c r="K9" t="s">
+        <v>4669</v>
+      </c>
+      <c r="L9" t="s">
         <v>4670</v>
-      </c>
-      <c r="L9" t="s">
-        <v>4671</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -78194,7 +78179,7 @@
         <v>1884</v>
       </c>
       <c r="K10" t="s">
-        <v>4725</v>
+        <v>4724</v>
       </c>
       <c r="L10" t="s">
         <v>4378</v>
@@ -78202,7 +78187,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -78223,7 +78208,7 @@
         <v>1884</v>
       </c>
       <c r="K11" t="s">
-        <v>4726</v>
+        <v>4725</v>
       </c>
       <c r="L11" t="s">
         <v>4378</v>
@@ -78231,7 +78216,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -78252,7 +78237,7 @@
         <v>1884</v>
       </c>
       <c r="K12" t="s">
-        <v>4727</v>
+        <v>4726</v>
       </c>
       <c r="L12" t="s">
         <v>4378</v>
@@ -78267,8 +78252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78314,7 +78299,7 @@
         <v>4117</v>
       </c>
       <c r="L1" t="s">
-        <v>4605</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -78436,10 +78421,10 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>4503</v>
+        <v>4502</v>
       </c>
       <c r="M5" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -78465,10 +78450,10 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>4505</v>
+        <v>4504</v>
       </c>
       <c r="M6" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -78494,10 +78479,10 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>4506</v>
+        <v>4505</v>
       </c>
       <c r="M7" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -78523,10 +78508,10 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>4504</v>
+        <v>4503</v>
       </c>
       <c r="M8" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -78552,15 +78537,15 @@
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>4507</v>
+        <v>4506</v>
       </c>
       <c r="M9" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -78584,15 +78569,15 @@
         <v>328</v>
       </c>
       <c r="K10" t="s">
-        <v>4532</v>
+        <v>4531</v>
       </c>
       <c r="M10" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -78616,15 +78601,15 @@
         <v>328</v>
       </c>
       <c r="K11" t="s">
-        <v>4533</v>
+        <v>4532</v>
       </c>
       <c r="M11" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -78648,15 +78633,15 @@
         <v>328</v>
       </c>
       <c r="K12" t="s">
+        <v>4533</v>
+      </c>
+      <c r="M12" t="s">
         <v>4534</v>
-      </c>
-      <c r="M12" t="s">
-        <v>4535</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -78680,15 +78665,15 @@
         <v>348</v>
       </c>
       <c r="K13" t="s">
-        <v>4545</v>
+        <v>4544</v>
       </c>
       <c r="M13" t="s">
-        <v>4554</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -78712,15 +78697,15 @@
         <v>348</v>
       </c>
       <c r="K14" t="s">
-        <v>4546</v>
+        <v>4545</v>
       </c>
       <c r="M14" t="s">
-        <v>4554</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -78744,15 +78729,15 @@
         <v>348</v>
       </c>
       <c r="K15" t="s">
-        <v>4547</v>
+        <v>4546</v>
       </c>
       <c r="M15" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -78776,15 +78761,15 @@
         <v>348</v>
       </c>
       <c r="K16" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
       <c r="M16" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -78808,15 +78793,15 @@
         <v>328</v>
       </c>
       <c r="K17" t="s">
-        <v>4549</v>
+        <v>4548</v>
       </c>
       <c r="M17" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -78840,15 +78825,15 @@
         <v>328</v>
       </c>
       <c r="K18" t="s">
-        <v>4550</v>
+        <v>4549</v>
       </c>
       <c r="M18" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -78872,15 +78857,15 @@
         <v>328</v>
       </c>
       <c r="K19" t="s">
-        <v>4551</v>
+        <v>4550</v>
       </c>
       <c r="M19" t="s">
-        <v>4554</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -78904,15 +78889,15 @@
         <v>348</v>
       </c>
       <c r="K20" t="s">
-        <v>4552</v>
+        <v>4551</v>
       </c>
       <c r="M20" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -78936,15 +78921,15 @@
         <v>348</v>
       </c>
       <c r="K21" t="s">
-        <v>4553</v>
+        <v>4552</v>
       </c>
       <c r="M21" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -78968,12 +78953,12 @@
         <v>3138</v>
       </c>
       <c r="M22" t="s">
-        <v>4678</v>
+        <v>4677</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -79000,10 +78985,10 @@
         <v>1536</v>
       </c>
       <c r="K23" t="s">
+        <v>4743</v>
+      </c>
+      <c r="M23" t="s">
         <v>4744</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4745</v>
       </c>
     </row>
   </sheetData>
@@ -79063,7 +79048,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -79090,15 +79075,15 @@
         <v>328</v>
       </c>
       <c r="K2" t="s">
-        <v>4539</v>
+        <v>4538</v>
       </c>
       <c r="L2" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -79125,15 +79110,15 @@
         <v>328</v>
       </c>
       <c r="K3" t="s">
+        <v>4539</v>
+      </c>
+      <c r="L3" t="s">
         <v>4540</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4541</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -79157,12 +79142,12 @@
         <v>2227</v>
       </c>
       <c r="L4" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -79186,12 +79171,12 @@
         <v>2229</v>
       </c>
       <c r="L5" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -79212,15 +79197,15 @@
         <v>186</v>
       </c>
       <c r="K6" t="s">
-        <v>4617</v>
+        <v>4616</v>
       </c>
       <c r="L6" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -79241,15 +79226,15 @@
         <v>186</v>
       </c>
       <c r="K7" t="s">
-        <v>4618</v>
+        <v>4617</v>
       </c>
       <c r="L7" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -79270,15 +79255,15 @@
         <v>186</v>
       </c>
       <c r="K8" t="s">
-        <v>4619</v>
+        <v>4618</v>
       </c>
       <c r="L8" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -79299,15 +79284,15 @@
         <v>186</v>
       </c>
       <c r="K9" t="s">
-        <v>4620</v>
+        <v>4619</v>
       </c>
       <c r="L9" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -79328,15 +79313,15 @@
         <v>186</v>
       </c>
       <c r="K10" t="s">
-        <v>4621</v>
+        <v>4620</v>
       </c>
       <c r="L10" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -79357,15 +79342,15 @@
         <v>186</v>
       </c>
       <c r="K11" t="s">
-        <v>4622</v>
+        <v>4621</v>
       </c>
       <c r="L11" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -79386,15 +79371,15 @@
         <v>186</v>
       </c>
       <c r="K12" t="s">
-        <v>4623</v>
+        <v>4622</v>
       </c>
       <c r="L12" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -79415,15 +79400,15 @@
         <v>186</v>
       </c>
       <c r="K13" t="s">
-        <v>4624</v>
+        <v>4623</v>
       </c>
       <c r="L13" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -79444,15 +79429,15 @@
         <v>186</v>
       </c>
       <c r="K14" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="L14" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -79473,15 +79458,15 @@
         <v>186</v>
       </c>
       <c r="K15" t="s">
-        <v>4626</v>
+        <v>4625</v>
       </c>
       <c r="L15" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -79499,15 +79484,15 @@
         <v>186</v>
       </c>
       <c r="K16" t="s">
-        <v>4616</v>
+        <v>4615</v>
       </c>
       <c r="L16" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -79530,15 +79515,15 @@
       </c>
       <c r="I17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="L17" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -79561,15 +79546,15 @@
       </c>
       <c r="I18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>4632</v>
+        <v>4631</v>
       </c>
       <c r="L18" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -79592,15 +79577,15 @@
       </c>
       <c r="I19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>4635</v>
+        <v>4634</v>
       </c>
       <c r="L19" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -79623,15 +79608,15 @@
       </c>
       <c r="I20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>4633</v>
+        <v>4632</v>
       </c>
       <c r="L20" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -79654,15 +79639,15 @@
       </c>
       <c r="I21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>4634</v>
+        <v>4633</v>
       </c>
       <c r="L21" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -79685,15 +79670,15 @@
       </c>
       <c r="I22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>4636</v>
+        <v>4635</v>
       </c>
       <c r="L22" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -79716,15 +79701,15 @@
       </c>
       <c r="I23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>4637</v>
+        <v>4636</v>
       </c>
       <c r="L23" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -79747,15 +79732,15 @@
       </c>
       <c r="I24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>4638</v>
+        <v>4637</v>
       </c>
       <c r="L24" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -79778,15 +79763,15 @@
       </c>
       <c r="I25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>4639</v>
+        <v>4638</v>
       </c>
       <c r="L25" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -79809,10 +79794,10 @@
       </c>
       <c r="I26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>4640</v>
+        <v>4639</v>
       </c>
       <c r="L26" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
     </row>
   </sheetData>
@@ -80012,7 +79997,7 @@
         <v>186</v>
       </c>
       <c r="L6" t="s">
-        <v>4579</v>
+        <v>4578</v>
       </c>
       <c r="M6" t="s">
         <v>4340</v>
@@ -80020,7 +80005,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -80047,15 +80032,15 @@
         <v>1536</v>
       </c>
       <c r="L7" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
       <c r="M7" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -80082,15 +80067,15 @@
         <v>328</v>
       </c>
       <c r="L8" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
       <c r="M8" t="s">
-        <v>4544</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -80117,15 +80102,15 @@
         <v>328</v>
       </c>
       <c r="L9" t="s">
+        <v>4542</v>
+      </c>
+      <c r="M9" t="s">
         <v>4543</v>
-      </c>
-      <c r="M9" t="s">
-        <v>4544</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -80149,15 +80134,15 @@
         <v>3179</v>
       </c>
       <c r="L10" t="s">
-        <v>4570</v>
+        <v>4569</v>
       </c>
       <c r="M10" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -80181,15 +80166,15 @@
         <v>3179</v>
       </c>
       <c r="L11" t="s">
-        <v>4571</v>
+        <v>4570</v>
       </c>
       <c r="M11" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -80213,15 +80198,15 @@
         <v>3179</v>
       </c>
       <c r="L12" t="s">
-        <v>4572</v>
+        <v>4571</v>
       </c>
       <c r="M12" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -80245,15 +80230,15 @@
         <v>3187</v>
       </c>
       <c r="L13" t="s">
-        <v>4573</v>
+        <v>4572</v>
       </c>
       <c r="M13" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -80277,15 +80262,15 @@
         <v>3187</v>
       </c>
       <c r="L14" t="s">
-        <v>4574</v>
+        <v>4573</v>
       </c>
       <c r="M14" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -80309,15 +80294,15 @@
         <v>3187</v>
       </c>
       <c r="L15" t="s">
-        <v>4575</v>
+        <v>4574</v>
       </c>
       <c r="M15" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -80341,15 +80326,15 @@
         <v>3187</v>
       </c>
       <c r="L16" t="s">
-        <v>4576</v>
+        <v>4575</v>
       </c>
       <c r="M16" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -80373,15 +80358,15 @@
         <v>3187</v>
       </c>
       <c r="L17" t="s">
-        <v>4577</v>
+        <v>4576</v>
       </c>
       <c r="M17" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -80405,15 +80390,15 @@
         <v>3187</v>
       </c>
       <c r="L18" t="s">
-        <v>4578</v>
+        <v>4577</v>
       </c>
       <c r="M18" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -80440,15 +80425,15 @@
         <v>1305</v>
       </c>
       <c r="L19" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="M19" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -80472,12 +80457,12 @@
         <v>509</v>
       </c>
       <c r="M20" t="s">
-        <v>4613</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -80501,12 +80486,12 @@
         <v>511</v>
       </c>
       <c r="M21" t="s">
-        <v>4614</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -80527,15 +80512,15 @@
         <v>1309</v>
       </c>
       <c r="L22" t="s">
-        <v>4647</v>
+        <v>4646</v>
       </c>
       <c r="M22" t="s">
-        <v>4649</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -80556,15 +80541,15 @@
         <v>1309</v>
       </c>
       <c r="L23" t="s">
+        <v>4647</v>
+      </c>
+      <c r="M23" t="s">
         <v>4648</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4649</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -80594,15 +80579,15 @@
         <v>180</v>
       </c>
       <c r="L24" t="s">
+        <v>4653</v>
+      </c>
+      <c r="M24" t="s">
         <v>4654</v>
-      </c>
-      <c r="M24" t="s">
-        <v>4655</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -80623,15 +80608,15 @@
         <v>514</v>
       </c>
       <c r="L25" t="s">
+        <v>4700</v>
+      </c>
+      <c r="M25" t="s">
         <v>4701</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4702</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -80652,15 +80637,15 @@
         <v>1884</v>
       </c>
       <c r="L26" t="s">
-        <v>4718</v>
+        <v>4717</v>
       </c>
       <c r="M26" t="s">
-        <v>4722</v>
+        <v>4721</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -80681,15 +80666,15 @@
         <v>1884</v>
       </c>
       <c r="L27" t="s">
-        <v>4719</v>
+        <v>4718</v>
       </c>
       <c r="M27" t="s">
-        <v>4723</v>
+        <v>4722</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -80710,15 +80695,15 @@
         <v>1884</v>
       </c>
       <c r="L28" t="s">
-        <v>4720</v>
+        <v>4719</v>
       </c>
       <c r="M28" t="s">
-        <v>4724</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -80739,15 +80724,15 @@
         <v>1884</v>
       </c>
       <c r="L29" t="s">
-        <v>4721</v>
+        <v>4720</v>
       </c>
       <c r="M29" t="s">
-        <v>4724</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -80771,15 +80756,15 @@
         <v>180</v>
       </c>
       <c r="L30" t="s">
-        <v>4765</v>
+        <v>4764</v>
       </c>
       <c r="M30" t="s">
-        <v>4769</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -80803,15 +80788,15 @@
         <v>180</v>
       </c>
       <c r="L31" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
       <c r="M31" t="s">
-        <v>4770</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -80835,15 +80820,15 @@
         <v>180</v>
       </c>
       <c r="L32" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="M32" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -80867,10 +80852,10 @@
         <v>180</v>
       </c>
       <c r="L33" t="s">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="M33" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
     </row>
   </sheetData>
@@ -81463,7 +81448,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -81487,12 +81472,12 @@
         <v>3187</v>
       </c>
       <c r="M22" t="s">
-        <v>4569</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -81519,12 +81504,12 @@
         <v>1305</v>
       </c>
       <c r="M23" t="s">
-        <v>4588</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -81545,12 +81530,12 @@
         <v>186</v>
       </c>
       <c r="M24" t="s">
-        <v>4606</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -81576,7 +81561,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -81605,7 +81590,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -81635,12 +81620,12 @@
         <v>180</v>
       </c>
       <c r="M27" t="s">
-        <v>4653</v>
+        <v>4652</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -81667,12 +81652,12 @@
         <v>180</v>
       </c>
       <c r="M28" t="s">
-        <v>4672</v>
+        <v>4671</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -81699,7 +81684,7 @@
         <v>3292</v>
       </c>
       <c r="M29" t="s">
-        <v>4693</v>
+        <v>4692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added m6805,i8039 cpu cores and alexkidda to system16 driver (sprite colours not correct)
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="4" r:id="rId1"/>
@@ -14963,10 +14963,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15310,27 +15310,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>4688</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>4581</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="M1" s="5" t="s">
         <v>4500</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15886,8 +15886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16179,8 +16179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1380" workbookViewId="0">
-      <selection activeCell="A835" sqref="A835:XFD836"/>
+    <sheetView topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="J389" sqref="J389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64413,7 +64413,7 @@
       <c r="B66">
         <v>65</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="4">
         <v>1942</v>
       </c>
       <c r="D66" t="s">
@@ -64670,7 +64670,7 @@
       <c r="B76">
         <v>75</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="4">
         <v>600</v>
       </c>
       <c r="D76" t="s">
@@ -64685,7 +64685,7 @@
       <c r="I76" t="s">
         <v>186</v>
       </c>
-      <c r="L76" s="5">
+      <c r="L76" s="4">
         <v>600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes to v30 . seems that all m72 games are playable now
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\arcadeflex036\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="794" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="status" sheetId="4" r:id="rId1"/>
@@ -27,7 +22,7 @@
   <definedNames>
     <definedName name="compatibility" localSheetId="10">compatibility.xls!$C$1:$AB$1444</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -15284,7 +15279,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15886,7 +15881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -16179,8 +16174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB1440"/>
   <sheetViews>
-    <sheetView topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="J389" sqref="J389"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="C365" sqref="C365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77332,7 +77327,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79564,8 +79559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>